<commit_message>
Add new script to fix chemkin files created with RMG's plog bug
See RMG-Py issue number 147. RMG used to print plog blocks incorrectly. This script takes these chemkin files and outputs a corrected one.
</commit_message>
<xml_diff>
--- a/Master_list.xlsx
+++ b/Master_list.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="192" uniqueCount="118">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="196" uniqueCount="120">
   <si>
     <t>Quick operations for one data point</t>
   </si>
@@ -381,6 +381,12 @@
   </si>
   <si>
     <t>Shows example of making a regression test on observables like concentration profiles or ignition delay</t>
+  </si>
+  <si>
+    <t>fixPlog.py</t>
+  </si>
+  <si>
+    <t>Converts a chemkin with erroneous duplicate plogs to the correct format *See RMG-Py issue 147</t>
   </si>
 </sst>
 </file>
@@ -715,10 +721,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D71"/>
+  <dimension ref="A1:D72"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A46" workbookViewId="0">
-      <selection activeCell="A67" sqref="A67"/>
+    <sheetView tabSelected="1" topLeftCell="B40" workbookViewId="0">
+      <selection activeCell="D49" sqref="D49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1229,42 +1235,42 @@
         <v>80</v>
       </c>
     </row>
-    <row r="50" spans="1:4" s="4" customFormat="1" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A50" s="3" t="s">
+    <row r="49" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A49" t="s">
+        <v>118</v>
+      </c>
+      <c r="B49" t="s">
+        <v>79</v>
+      </c>
+      <c r="C49" t="s">
+        <v>34</v>
+      </c>
+      <c r="D49" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="51" spans="1:4" s="4" customFormat="1" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A51" s="3" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="51" spans="1:4" s="4" customFormat="1" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A51" s="4" t="s">
+    <row r="52" spans="1:4" s="4" customFormat="1" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A52" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="B51" s="4" t="s">
+      <c r="B52" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="C51" s="4" t="s">
+      <c r="C52" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="D51" s="4" t="s">
+      <c r="D52" s="4" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A52" s="2" t="s">
+    <row r="53" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A53" s="2" t="s">
         <v>82</v>
-      </c>
-      <c r="B52" t="s">
-        <v>3</v>
-      </c>
-      <c r="C52" t="s">
-        <v>33</v>
-      </c>
-      <c r="D52" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A53" t="s">
-        <v>83</v>
       </c>
       <c r="B53" t="s">
         <v>3</v>
@@ -1273,158 +1279,172 @@
         <v>33</v>
       </c>
       <c r="D53" t="s">
-        <v>84</v>
+        <v>115</v>
       </c>
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="B54" t="s">
-        <v>87</v>
+        <v>3</v>
+      </c>
+      <c r="C54" t="s">
+        <v>33</v>
       </c>
       <c r="D54" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="B55" t="s">
-        <v>18</v>
+        <v>87</v>
       </c>
       <c r="D55" t="s">
-        <v>116</v>
+        <v>86</v>
       </c>
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B56" t="s">
-        <v>90</v>
-      </c>
-      <c r="C56" t="s">
-        <v>34</v>
+        <v>18</v>
       </c>
       <c r="D56" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="B57" t="s">
-        <v>3</v>
+        <v>90</v>
       </c>
       <c r="C57" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="D57" t="s">
-        <v>92</v>
+        <v>117</v>
       </c>
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
+        <v>91</v>
+      </c>
+      <c r="B58" t="s">
+        <v>3</v>
+      </c>
+      <c r="C58" t="s">
+        <v>33</v>
+      </c>
+      <c r="D58" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="59" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A59" t="s">
         <v>94</v>
       </c>
-      <c r="B58" t="s">
+      <c r="B59" t="s">
         <v>93</v>
       </c>
-      <c r="C58" t="s">
+      <c r="C59" t="s">
         <v>37</v>
       </c>
-      <c r="D58" t="s">
+      <c r="D59" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="60" spans="1:4" s="4" customFormat="1" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A60" s="3" t="s">
+    <row r="61" spans="1:4" s="4" customFormat="1" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A61" s="3" t="s">
         <v>96</v>
       </c>
     </row>
-    <row r="61" spans="1:4" s="4" customFormat="1" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A61" s="4" t="s">
+    <row r="62" spans="1:4" s="4" customFormat="1" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A62" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="B61" s="4" t="s">
+      <c r="B62" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="C61" s="4" t="s">
+      <c r="C62" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="D61" s="4" t="s">
+      <c r="D62" s="4" t="s">
         <v>22</v>
-      </c>
-    </row>
-    <row r="62" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A62" t="s">
-        <v>97</v>
-      </c>
-      <c r="B62" t="s">
-        <v>98</v>
-      </c>
-      <c r="C62" t="s">
-        <v>99</v>
-      </c>
-      <c r="D62" t="s">
-        <v>100</v>
       </c>
     </row>
     <row r="63" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A63" t="s">
+        <v>97</v>
+      </c>
+      <c r="B63" t="s">
+        <v>98</v>
+      </c>
+      <c r="C63" t="s">
+        <v>99</v>
+      </c>
+      <c r="D63" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="64" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A64" t="s">
         <v>101</v>
       </c>
-      <c r="B63" t="s">
+      <c r="B64" t="s">
         <v>102</v>
       </c>
-      <c r="D63" t="s">
+      <c r="D64" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="65" spans="1:4" s="4" customFormat="1" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A65" s="3" t="s">
+    <row r="66" spans="1:4" s="4" customFormat="1" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A66" s="3" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="66" spans="1:4" s="4" customFormat="1" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A66" s="4" t="s">
+    <row r="67" spans="1:4" s="4" customFormat="1" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A67" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="B66" s="4" t="s">
+      <c r="B67" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="C66" s="4" t="s">
+      <c r="C67" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="D66" s="4" t="s">
+      <c r="D67" s="4" t="s">
         <v>22</v>
-      </c>
-    </row>
-    <row r="67" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A67" t="s">
-        <v>105</v>
       </c>
     </row>
     <row r="68" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A68" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
     <row r="69" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A69" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="70" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A70" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
     </row>
     <row r="71" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A71" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="72" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A72" t="s">
         <v>109</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Added Chemkin FITDAT utility to list of useful scripts
</commit_message>
<xml_diff>
--- a/Master_list.xlsx
+++ b/Master_list.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="205" uniqueCount="125">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="208" uniqueCount="128">
   <si>
     <t>Quick operations for one data point</t>
   </si>
@@ -396,6 +396,16 @@
   <si>
     <t>Fits a csv table of k(T,P) values to a Chebyshev polynomial using Cantherm's built-in functions and outputs the fit k in 
 Chemkin format</t>
+  </si>
+  <si>
+    <t>This tool already exists in Chemkin as the FITDAT utility</t>
+  </si>
+  <si>
+    <t>Chemkin</t>
+  </si>
+  <si>
+    <t>Fits thermo data in a variety of forms to different polynomials used in Chemkin.
+Refer to Chapter 7 of the Chemkin Input manual for instructions</t>
   </si>
 </sst>
 </file>
@@ -722,7 +732,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -733,7 +743,7 @@
   <dimension ref="A1:D76"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A61" workbookViewId="0">
-      <selection activeCell="C69" sqref="C69"/>
+      <selection activeCell="A77" sqref="A77"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -1486,9 +1496,18 @@
         <v>107</v>
       </c>
     </row>
-    <row r="76" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:4" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
         <v>108</v>
+      </c>
+      <c r="B76" t="s">
+        <v>125</v>
+      </c>
+      <c r="C76" t="s">
+        <v>126</v>
+      </c>
+      <c r="D76" s="1" t="s">
+        <v>127</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add script findSpeciesInDictionary which outputs RMG names for inputted species
</commit_message>
<xml_diff>
--- a/Master_list.xlsx
+++ b/Master_list.xlsx
@@ -1,21 +1,33 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="Calc"/>
-  <workbookPr backupFile="false" showObjects="all" date1904="false"/>
-  <workbookProtection/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="27610"/>
+  <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Nate/code/Work-In-Progress_scripts/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16000" tabRatio="500"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId2"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
+  <calcPr calcId="0" iterateDelta="1E-4" concurrentCalc="0"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
+      <x14:workbookPr defaultImageDpi="32767"/>
+    </ext>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="225" uniqueCount="136">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="229" uniqueCount="138">
   <si>
     <t>Quick operations for one data point</t>
   </si>
@@ -227,7 +239,7 @@
     <t>Convert AdjList</t>
   </si>
   <si>
-    <t>Converts a new style adjList to an old style </t>
+    <t>Converts a new style adjList to an old style</t>
   </si>
   <si>
     <t>Convert old style adjlist to a new style</t>
@@ -275,7 +287,7 @@
     <t>Nate, Zach</t>
   </si>
   <si>
-    <t>Creates an input file taking output concentrationsfrom previously completed RMG-job </t>
+    <t>Creates an input file taking output concentrationsfrom previously completed RMG-job</t>
   </si>
   <si>
     <t>Modifying chemkin.inp</t>
@@ -426,16 +438,19 @@
   <si>
     <t>Fits thermo data in a variety of forms to different polynomials used in Chemkin.
 Refer to Chapter 7 of the Chemkin Input manual for instructions</t>
+  </si>
+  <si>
+    <t>findSpeciesInDictionary</t>
+  </si>
+  <si>
+    <t>Gives RMG name for species from an inputted RMG-dictionary from a list of SMILES</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="GENERAL"/>
-  </numFmts>
-  <fonts count="5">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color rgb="FF000000"/>
@@ -444,22 +459,7 @@
       <charset val="1"/>
     </font>
     <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="0"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="0"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="0"/>
-    </font>
-    <font>
-      <b val="true"/>
+      <b/>
       <sz val="12"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
@@ -482,7 +482,7 @@
     </fill>
   </fills>
   <borders count="1">
-    <border diagonalUp="false" diagonalDown="false">
+    <border>
       <left/>
       <right/>
       <top/>
@@ -490,61 +490,23 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="20">
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="41" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+  <cellStyleXfs count="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="5">
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="6">
-    <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="false"/>
-    <cellStyle name="Comma" xfId="15" builtinId="3" customBuiltin="false"/>
-    <cellStyle name="Comma [0]" xfId="16" builtinId="6" customBuiltin="false"/>
-    <cellStyle name="Currency" xfId="17" builtinId="4" customBuiltin="false"/>
-    <cellStyle name="Currency [0]" xfId="18" builtinId="7" customBuiltin="false"/>
-    <cellStyle name="Percent" xfId="19" builtinId="5" customBuiltin="false"/>
+  <cellStyles count="1">
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
+  <dxfs count="0"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium7"/>
   <colors>
     <indexedColors>
       <rgbColor rgb="FF000000"/>
@@ -603,37 +565,305 @@
       <rgbColor rgb="FF993366"/>
       <rgbColor rgb="FF333399"/>
       <rgbColor rgb="FF333333"/>
+      <rgbColor rgb="00003366"/>
+      <rgbColor rgb="00339966"/>
+      <rgbColor rgb="00003300"/>
+      <rgbColor rgb="00333300"/>
+      <rgbColor rgb="00993300"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00333399"/>
+      <rgbColor rgb="00333333"/>
     </indexedColors>
   </colors>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
+<file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+  <a:themeElements>
+    <a:clrScheme name="Office">
+      <a:dk1>
+        <a:sysClr val="windowText" lastClr="000000"/>
+      </a:dk1>
+      <a:lt1>
+        <a:sysClr val="window" lastClr="FFFFFF"/>
+      </a:lt1>
+      <a:dk2>
+        <a:srgbClr val="44546A"/>
+      </a:dk2>
+      <a:lt2>
+        <a:srgbClr val="E7E6E6"/>
+      </a:lt2>
+      <a:accent1>
+        <a:srgbClr val="5B9BD5"/>
+      </a:accent1>
+      <a:accent2>
+        <a:srgbClr val="ED7D31"/>
+      </a:accent2>
+      <a:accent3>
+        <a:srgbClr val="A5A5A5"/>
+      </a:accent3>
+      <a:accent4>
+        <a:srgbClr val="FFC000"/>
+      </a:accent4>
+      <a:accent5>
+        <a:srgbClr val="4472C4"/>
+      </a:accent5>
+      <a:accent6>
+        <a:srgbClr val="70AD47"/>
+      </a:accent6>
+      <a:hlink>
+        <a:srgbClr val="0563C1"/>
+      </a:hlink>
+      <a:folHlink>
+        <a:srgbClr val="954F72"/>
+      </a:folHlink>
+    </a:clrScheme>
+    <a:fontScheme name="Office">
+      <a:majorFont>
+        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:ea typeface=""/>
+        <a:cs typeface=""/>
+        <a:font script="Jpan" typeface="Yu Gothic Light"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="DengXian Light"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Times New Roman"/>
+        <a:font script="Hebr" typeface="Times New Roman"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="MoolBoran"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Times New Roman"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+      </a:majorFont>
+      <a:minorFont>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:ea typeface=""/>
+        <a:cs typeface=""/>
+        <a:font script="Jpan" typeface="Yu Gothic"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="DengXian"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Arial"/>
+        <a:font script="Hebr" typeface="Arial"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="DaunPenh"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Arial"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+      </a:minorFont>
+    </a:fontScheme>
+    <a:fmtScheme name="Office">
+      <a:fillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="110000"/>
+                <a:satMod val="105000"/>
+                <a:tint val="67000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="50000">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="105000"/>
+                <a:satMod val="103000"/>
+                <a:tint val="73000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="105000"/>
+                <a:satMod val="109000"/>
+                <a:tint val="81000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="0"/>
+        </a:gradFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:satMod val="103000"/>
+                <a:lumMod val="102000"/>
+                <a:tint val="94000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="50000">
+              <a:schemeClr val="phClr">
+                <a:satMod val="110000"/>
+                <a:lumMod val="100000"/>
+                <a:shade val="100000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="99000"/>
+                <a:satMod val="120000"/>
+                <a:shade val="78000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="0"/>
+        </a:gradFill>
+      </a:fillStyleLst>
+      <a:lnStyleLst>
+        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+        <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+        <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+      </a:lnStyleLst>
+      <a:effectStyleLst>
+        <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst>
+            <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="63000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
+        </a:effectStyle>
+      </a:effectStyleLst>
+      <a:bgFillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:solidFill>
+          <a:schemeClr val="phClr">
+            <a:tint val="95000"/>
+            <a:satMod val="170000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:tint val="93000"/>
+                <a:satMod val="150000"/>
+                <a:shade val="98000"/>
+                <a:lumMod val="102000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="50000">
+              <a:schemeClr val="phClr">
+                <a:tint val="98000"/>
+                <a:satMod val="130000"/>
+                <a:shade val="90000"/>
+                <a:lumMod val="103000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:shade val="63000"/>
+                <a:satMod val="120000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="0"/>
+        </a:gradFill>
+      </a:bgFillStyleLst>
+    </a:fmtScheme>
+  </a:themeElements>
+  <a:objectDefaults/>
+  <a:extraClrSchemeLst/>
+  <a:extLst>
+    <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+    </a:ext>
+  </a:extLst>
+</a:theme>
+</file>
+
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
-  </sheetPr>
-  <dimension ref="A1:D80"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:D81"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D22" sqref="D22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="16"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="67"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="66.8333333333333"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="31.5"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="100.503703703704"/>
-    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="11"/>
+    <col min="1" max="1" width="66.1640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="109.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" s="2" customFormat="true" ht="17" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="1" spans="1:4" s="2" customFormat="1" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
@@ -647,96 +877,96 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="0" t="s">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
         <v>5</v>
       </c>
-      <c r="B3" s="0" t="s">
+      <c r="B3" t="s">
         <v>6</v>
       </c>
-      <c r="C3" s="0" t="s">
+      <c r="C3" t="s">
         <v>7</v>
       </c>
       <c r="D3" s="3" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="4" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="0" t="s">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
         <v>9</v>
       </c>
-      <c r="B4" s="0" t="s">
+      <c r="B4" t="s">
         <v>6</v>
       </c>
-      <c r="C4" s="0" t="s">
+      <c r="C4" t="s">
         <v>7</v>
       </c>
-      <c r="D4" s="0" t="s">
+      <c r="D4" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="5" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="0" t="s">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
         <v>11</v>
       </c>
-      <c r="B5" s="0" t="s">
+      <c r="B5" t="s">
         <v>6</v>
       </c>
-      <c r="C5" s="0" t="s">
+      <c r="C5" t="s">
         <v>7</v>
       </c>
-      <c r="D5" s="0" t="s">
+      <c r="D5" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="6" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="0" t="s">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
         <v>13</v>
       </c>
-      <c r="B6" s="0" t="s">
+      <c r="B6" t="s">
         <v>6</v>
       </c>
-      <c r="C6" s="0" t="s">
+      <c r="C6" t="s">
         <v>7</v>
       </c>
-      <c r="D6" s="0" t="s">
+      <c r="D6" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="7" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="0" t="s">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
         <v>15</v>
       </c>
-      <c r="B7" s="0" t="s">
+      <c r="B7" t="s">
         <v>16</v>
       </c>
-      <c r="C7" s="0" t="s">
+      <c r="C7" t="s">
         <v>17</v>
       </c>
-      <c r="D7" s="0" t="s">
+      <c r="D7" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="8" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="0" t="s">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
         <v>19</v>
       </c>
-      <c r="B8" s="0" t="s">
+      <c r="B8" t="s">
         <v>16</v>
       </c>
-      <c r="C8" s="0" t="s">
+      <c r="C8" t="s">
         <v>17</v>
       </c>
-      <c r="D8" s="0" t="s">
+      <c r="D8" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="10" s="2" customFormat="true" ht="17" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="10" spans="1:4" s="2" customFormat="1" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="11" customFormat="false" ht="17" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="11" spans="1:4" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="2" t="s">
         <v>1</v>
       </c>
@@ -750,118 +980,118 @@
         <v>4</v>
       </c>
     </row>
-    <row r="12" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="0" t="s">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
         <v>22</v>
       </c>
-      <c r="B12" s="0" t="s">
+      <c r="B12" t="s">
         <v>23</v>
       </c>
-      <c r="D12" s="0" t="s">
+      <c r="D12" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="13" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="0" t="s">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
         <v>25</v>
       </c>
-      <c r="B13" s="0" t="s">
+      <c r="B13" t="s">
         <v>6</v>
       </c>
-      <c r="C13" s="0" t="s">
+      <c r="C13" t="s">
         <v>7</v>
       </c>
-      <c r="D13" s="0" t="s">
+      <c r="D13" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="14" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="0" t="s">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
         <v>27</v>
       </c>
-      <c r="B14" s="0" t="s">
+      <c r="B14" t="s">
         <v>23</v>
       </c>
-      <c r="D14" s="0" t="s">
+      <c r="D14" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="15" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="0" t="s">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
         <v>29</v>
       </c>
-      <c r="B15" s="0" t="s">
+      <c r="B15" t="s">
         <v>30</v>
       </c>
-      <c r="C15" s="0" t="s">
+      <c r="C15" t="s">
         <v>7</v>
       </c>
-      <c r="D15" s="0" t="s">
+      <c r="D15" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="0" t="s">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
         <v>32</v>
       </c>
-      <c r="B16" s="0" t="s">
+      <c r="B16" t="s">
         <v>30</v>
       </c>
-      <c r="C16" s="0" t="s">
+      <c r="C16" t="s">
         <v>7</v>
       </c>
-      <c r="D16" s="0" t="s">
+      <c r="D16" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="0" t="s">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
         <v>34</v>
       </c>
-      <c r="B17" s="0" t="s">
+      <c r="B17" t="s">
         <v>30</v>
       </c>
-      <c r="C17" s="0" t="s">
+      <c r="C17" t="s">
         <v>7</v>
       </c>
-      <c r="D17" s="0" t="s">
+      <c r="D17" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="0" t="s">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A18" t="s">
         <v>36</v>
       </c>
-      <c r="B18" s="0" t="s">
+      <c r="B18" t="s">
         <v>30</v>
       </c>
-      <c r="C18" s="0" t="s">
+      <c r="C18" t="s">
         <v>7</v>
       </c>
-      <c r="D18" s="0" t="s">
+      <c r="D18" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="0" t="s">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A19" t="s">
         <v>38</v>
       </c>
-      <c r="B19" s="0" t="s">
+      <c r="B19" t="s">
         <v>30</v>
       </c>
-      <c r="C19" s="0" t="s">
+      <c r="C19" t="s">
         <v>7</v>
       </c>
-      <c r="D19" s="0" t="s">
+      <c r="D19" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="21" s="2" customFormat="true" ht="17" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="21" spans="1:4" s="2" customFormat="1" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21" s="1" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="22" customFormat="false" ht="17" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="22" spans="1:4" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A22" s="2" t="s">
         <v>1</v>
       </c>
@@ -875,581 +1105,590 @@
         <v>4</v>
       </c>
     </row>
-    <row r="23" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="0" t="s">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A23" t="s">
         <v>41</v>
       </c>
-      <c r="B23" s="0" t="s">
+      <c r="B23" t="s">
         <v>42</v>
       </c>
-      <c r="C23" s="0" t="s">
+      <c r="C23" t="s">
         <v>17</v>
       </c>
-      <c r="D23" s="0" t="s">
+      <c r="D23" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="24" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A24" s="0" t="s">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A24" t="s">
         <v>44</v>
       </c>
-      <c r="B24" s="0" t="s">
+      <c r="B24" t="s">
         <v>45</v>
       </c>
-      <c r="C24" s="0" t="s">
+      <c r="C24" t="s">
         <v>17</v>
       </c>
-      <c r="D24" s="0" t="s">
+      <c r="D24" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="26" s="2" customFormat="true" ht="17" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A26" s="1" t="s">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A25" t="s">
+        <v>136</v>
+      </c>
+      <c r="B25" t="s">
+        <v>56</v>
+      </c>
+      <c r="C25" t="s">
+        <v>17</v>
+      </c>
+      <c r="D25" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" s="2" customFormat="1" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A27" s="1" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="27" customFormat="false" ht="17" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A27" s="2" t="s">
+    <row r="28" spans="1:4" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A28" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B27" s="2" t="s">
+      <c r="B28" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="C27" s="2" t="s">
+      <c r="C28" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="D27" s="2" t="s">
+      <c r="D28" s="2" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="28" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A28" s="0" t="s">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A29" t="s">
         <v>48</v>
       </c>
-      <c r="B28" s="0" t="s">
+      <c r="B29" t="s">
         <v>49</v>
       </c>
-      <c r="C28" s="0" t="s">
+      <c r="C29" t="s">
         <v>50</v>
       </c>
-      <c r="D28" s="0" t="s">
+      <c r="D29" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="29" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A29" s="0" t="s">
+    <row r="30" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A30" t="s">
         <v>52</v>
       </c>
-      <c r="B29" s="0" t="s">
+      <c r="B30" t="s">
         <v>23</v>
       </c>
-      <c r="C29" s="0" t="s">
+      <c r="C30" t="s">
         <v>53</v>
       </c>
-      <c r="D29" s="0" t="s">
+      <c r="D30" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="30" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A30" s="0" t="s">
+    <row r="31" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A31" t="s">
         <v>55</v>
       </c>
-      <c r="B30" s="0" t="s">
+      <c r="B31" t="s">
         <v>56</v>
       </c>
-      <c r="C30" s="0" t="s">
+      <c r="C31" t="s">
         <v>17</v>
       </c>
-      <c r="D30" s="0" t="s">
+      <c r="D31" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="31" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A31" s="0" t="s">
+    <row r="32" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A32" t="s">
         <v>58</v>
       </c>
-      <c r="B31" s="0" t="s">
+      <c r="B32" t="s">
         <v>59</v>
       </c>
-      <c r="C31" s="0" t="s">
+      <c r="C32" t="s">
         <v>60</v>
       </c>
-      <c r="D31" s="0" t="s">
+      <c r="D32" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="32" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A32" s="0" t="s">
+    <row r="33" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A33" t="s">
         <v>62</v>
       </c>
-      <c r="B32" s="0" t="s">
+      <c r="B33" t="s">
         <v>63</v>
       </c>
-      <c r="D32" s="0" t="s">
+      <c r="D33" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="33" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A33" s="0" t="s">
+    <row r="34" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A34" t="s">
         <v>65</v>
       </c>
-      <c r="B33" s="0" t="s">
+      <c r="B34" t="s">
         <v>66</v>
       </c>
-      <c r="D33" s="0" t="s">
+      <c r="D34" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="35" s="2" customFormat="true" ht="17" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A35" s="1" t="s">
+    <row r="36" spans="1:4" s="2" customFormat="1" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A36" s="1" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="36" customFormat="false" ht="17" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A36" s="2" t="s">
+    <row r="37" spans="1:4" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A37" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B36" s="2" t="s">
+      <c r="B37" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="C36" s="2" t="s">
+      <c r="C37" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="D36" s="2" t="s">
+      <c r="D37" s="2" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="37" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A37" s="0" t="s">
+    <row r="38" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A38" t="s">
         <v>69</v>
       </c>
-      <c r="B37" s="0" t="s">
+      <c r="B38" t="s">
         <v>6</v>
       </c>
-      <c r="C37" s="0" t="s">
+      <c r="C38" t="s">
         <v>7</v>
       </c>
-      <c r="D37" s="0" t="s">
+      <c r="D38" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="38" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A38" s="0" t="s">
+    <row r="39" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A39" t="s">
         <v>5</v>
       </c>
-      <c r="B38" s="0" t="s">
+      <c r="B39" t="s">
         <v>6</v>
       </c>
-      <c r="C38" s="0" t="s">
+      <c r="C39" t="s">
         <v>7</v>
       </c>
-      <c r="D38" s="0" t="s">
+      <c r="D39" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="39" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A39" s="0" t="s">
+    <row r="40" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A40" t="s">
         <v>72</v>
       </c>
-      <c r="B39" s="0" t="s">
+      <c r="B40" t="s">
         <v>63</v>
       </c>
-      <c r="D39" s="0" t="s">
+      <c r="D40" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="40" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A40" s="0" t="s">
+    <row r="41" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A41" t="s">
         <v>74</v>
       </c>
-      <c r="B40" s="0" t="s">
+      <c r="B41" t="s">
         <v>63</v>
       </c>
-      <c r="D40" s="0" t="s">
+      <c r="D41" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="41" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A41" s="0" t="s">
+    <row r="42" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A42" t="s">
         <v>76</v>
       </c>
-      <c r="B41" s="0" t="s">
+      <c r="B42" t="s">
         <v>56</v>
       </c>
-      <c r="C41" s="0" t="s">
+      <c r="C42" t="s">
         <v>7</v>
       </c>
-      <c r="D41" s="0" t="s">
+      <c r="D42" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="43" s="2" customFormat="true" ht="17" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A43" s="1" t="s">
+    <row r="44" spans="1:4" s="2" customFormat="1" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A44" s="1" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="44" customFormat="false" ht="17" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A44" s="2" t="s">
+    <row r="45" spans="1:4" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A45" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B44" s="2" t="s">
+      <c r="B45" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="C44" s="2" t="s">
+      <c r="C45" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="D44" s="2" t="s">
+      <c r="D45" s="2" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="45" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A45" s="0" t="s">
+    <row r="46" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A46" t="s">
         <v>79</v>
       </c>
-      <c r="B45" s="0" t="s">
+      <c r="B46" t="s">
         <v>30</v>
       </c>
-      <c r="C45" s="0" t="s">
+      <c r="C46" t="s">
         <v>7</v>
       </c>
-      <c r="D45" s="0" t="s">
+      <c r="D46" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="46" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A46" s="0" t="s">
+    <row r="47" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A47" t="s">
         <v>81</v>
       </c>
-      <c r="B46" s="0" t="s">
+      <c r="B47" t="s">
         <v>30</v>
       </c>
-      <c r="C46" s="0" t="s">
+      <c r="C47" t="s">
         <v>17</v>
       </c>
-      <c r="D46" s="0" t="s">
+      <c r="D47" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="47" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A47" s="0" t="s">
+    <row r="48" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A48" t="s">
         <v>83</v>
       </c>
-      <c r="B47" s="0" t="s">
+      <c r="B48" t="s">
         <v>84</v>
       </c>
-      <c r="C47" s="0" t="s">
+      <c r="C48" t="s">
         <v>85</v>
       </c>
-      <c r="D47" s="0" t="s">
+      <c r="D48" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="49" s="2" customFormat="true" ht="17" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A49" s="1" t="s">
+    <row r="50" spans="1:4" s="2" customFormat="1" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A50" s="1" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="50" customFormat="false" ht="17" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A50" s="2" t="s">
+    <row r="51" spans="1:4" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A51" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B50" s="2" t="s">
+      <c r="B51" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="C50" s="2" t="s">
+      <c r="C51" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="D50" s="2" t="s">
+      <c r="D51" s="2" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="51" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A51" s="0" t="s">
+    <row r="52" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A52" t="s">
         <v>88</v>
       </c>
-      <c r="B51" s="0" t="s">
+      <c r="B52" t="s">
         <v>89</v>
       </c>
-      <c r="D51" s="0" t="s">
+      <c r="D52" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="52" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A52" s="0" t="s">
+    <row r="53" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A53" t="s">
         <v>91</v>
       </c>
-      <c r="B52" s="0" t="s">
+      <c r="B53" t="s">
         <v>92</v>
       </c>
-      <c r="C52" s="0" t="s">
+      <c r="C53" t="s">
         <v>17</v>
       </c>
-      <c r="D52" s="0" t="s">
+      <c r="D53" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="53" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A53" s="0" t="s">
+    <row r="54" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A54" t="s">
         <v>94</v>
       </c>
-      <c r="B53" s="0" t="s">
+      <c r="B54" t="s">
         <v>92</v>
       </c>
-      <c r="C53" s="0" t="s">
+      <c r="C54" t="s">
         <v>17</v>
       </c>
-      <c r="D53" s="0" t="s">
+      <c r="D54" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="55" s="2" customFormat="true" ht="17" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A55" s="1" t="s">
+    <row r="56" spans="1:4" s="2" customFormat="1" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A56" s="1" t="s">
         <v>96</v>
       </c>
     </row>
-    <row r="56" customFormat="false" ht="17" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A56" s="2" t="s">
+    <row r="57" spans="1:4" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A57" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B56" s="2" t="s">
+      <c r="B57" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="C56" s="2" t="s">
+      <c r="C57" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="D56" s="2" t="s">
+      <c r="D57" s="2" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="57" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A57" s="4" t="s">
+    <row r="58" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A58" s="4" t="s">
         <v>97</v>
       </c>
-      <c r="B57" s="0" t="s">
+      <c r="B58" t="s">
         <v>6</v>
       </c>
-      <c r="C57" s="0" t="s">
+      <c r="C58" t="s">
         <v>7</v>
       </c>
-      <c r="D57" s="0" t="s">
+      <c r="D58" t="s">
         <v>98</v>
       </c>
     </row>
-    <row r="58" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A58" s="0" t="s">
+    <row r="59" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A59" t="s">
         <v>99</v>
       </c>
-      <c r="B58" s="0" t="s">
+      <c r="B59" t="s">
         <v>6</v>
       </c>
-      <c r="C58" s="0" t="s">
+      <c r="C59" t="s">
         <v>7</v>
       </c>
-      <c r="D58" s="0" t="s">
+      <c r="D59" t="s">
         <v>100</v>
       </c>
     </row>
-    <row r="59" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A59" s="0" t="s">
+    <row r="60" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A60" t="s">
         <v>101</v>
       </c>
-      <c r="B59" s="0" t="s">
+      <c r="B60" t="s">
         <v>102</v>
       </c>
-      <c r="D59" s="0" t="s">
+      <c r="D60" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="60" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A60" s="0" t="s">
+    <row r="61" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A61" t="s">
         <v>104</v>
       </c>
-      <c r="B60" s="0" t="s">
+      <c r="B61" t="s">
         <v>23</v>
       </c>
-      <c r="D60" s="0" t="s">
+      <c r="D61" t="s">
         <v>105</v>
       </c>
     </row>
-    <row r="61" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A61" s="0" t="s">
+    <row r="62" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A62" t="s">
         <v>106</v>
       </c>
-      <c r="B61" s="0" t="s">
+      <c r="B62" t="s">
         <v>107</v>
       </c>
-      <c r="C61" s="0" t="s">
+      <c r="C62" t="s">
         <v>17</v>
       </c>
-      <c r="D61" s="0" t="s">
+      <c r="D62" t="s">
         <v>108</v>
       </c>
     </row>
-    <row r="62" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A62" s="0" t="s">
+    <row r="63" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A63" t="s">
         <v>109</v>
       </c>
-      <c r="B62" s="0" t="s">
+      <c r="B63" t="s">
         <v>6</v>
       </c>
-      <c r="C62" s="0" t="s">
+      <c r="C63" t="s">
         <v>7</v>
       </c>
-      <c r="D62" s="0" t="s">
+      <c r="D63" t="s">
         <v>110</v>
       </c>
     </row>
-    <row r="63" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A63" s="0" t="s">
+    <row r="64" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A64" t="s">
         <v>111</v>
       </c>
-      <c r="B63" s="0" t="s">
+      <c r="B64" t="s">
         <v>112</v>
       </c>
-      <c r="C63" s="0" t="s">
+      <c r="C64" t="s">
         <v>53</v>
       </c>
-      <c r="D63" s="0" t="s">
+      <c r="D64" t="s">
         <v>113</v>
       </c>
     </row>
-    <row r="65" s="2" customFormat="true" ht="17" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A65" s="1" t="s">
+    <row r="66" spans="1:4" s="2" customFormat="1" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A66" s="1" t="s">
         <v>114</v>
       </c>
     </row>
-    <row r="66" customFormat="false" ht="17" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A66" s="2" t="s">
+    <row r="67" spans="1:4" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A67" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B66" s="2" t="s">
+      <c r="B67" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="C66" s="2" t="s">
+      <c r="C67" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="D66" s="2" t="s">
+      <c r="D67" s="2" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="67" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A67" s="0" t="s">
+    <row r="68" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A68" t="s">
         <v>115</v>
       </c>
-      <c r="B67" s="0" t="s">
+      <c r="B68" t="s">
         <v>116</v>
       </c>
-      <c r="C67" s="0" t="s">
+      <c r="C68" t="s">
         <v>117</v>
       </c>
-      <c r="D67" s="0" t="s">
+      <c r="D68" t="s">
         <v>118</v>
       </c>
     </row>
-    <row r="68" customFormat="false" ht="32" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A68" s="0" t="s">
+    <row r="69" spans="1:4" ht="32" x14ac:dyDescent="0.2">
+      <c r="A69" t="s">
         <v>119</v>
       </c>
-      <c r="B68" s="0" t="s">
+      <c r="B69" t="s">
         <v>120</v>
       </c>
-      <c r="D68" s="3" t="s">
+      <c r="D69" s="3" t="s">
         <v>121</v>
       </c>
     </row>
-    <row r="70" s="2" customFormat="true" ht="17" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A70" s="1" t="s">
+    <row r="71" spans="1:4" s="2" customFormat="1" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A71" s="1" t="s">
         <v>122</v>
       </c>
     </row>
-    <row r="71" customFormat="false" ht="17" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A71" s="2" t="s">
+    <row r="72" spans="1:4" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A72" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B71" s="2" t="s">
+      <c r="B72" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="C71" s="2" t="s">
+      <c r="C72" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="D71" s="2" t="s">
+      <c r="D72" s="2" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="72" customFormat="false" ht="32" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A72" s="0" t="s">
+    <row r="73" spans="1:4" ht="32" x14ac:dyDescent="0.2">
+      <c r="A73" t="s">
         <v>123</v>
       </c>
-      <c r="B72" s="0" t="s">
+      <c r="B73" t="s">
         <v>124</v>
       </c>
-      <c r="C72" s="0" t="s">
+      <c r="C73" t="s">
         <v>125</v>
       </c>
-      <c r="D72" s="3" t="s">
+      <c r="D73" s="3" t="s">
         <v>126</v>
       </c>
     </row>
-    <row r="74" s="2" customFormat="true" ht="17" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A74" s="1" t="s">
+    <row r="75" spans="1:4" s="2" customFormat="1" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A75" s="1" t="s">
         <v>127</v>
       </c>
     </row>
-    <row r="75" customFormat="false" ht="17" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A75" s="2" t="s">
+    <row r="76" spans="1:4" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A76" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B75" s="2" t="s">
+      <c r="B76" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="C75" s="2" t="s">
+      <c r="C76" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="D75" s="2" t="s">
+      <c r="D76" s="2" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="76" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A76" s="0" t="s">
+    <row r="77" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A77" t="s">
         <v>128</v>
       </c>
     </row>
-    <row r="77" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A77" s="0" t="s">
+    <row r="78" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A78" t="s">
         <v>129</v>
       </c>
     </row>
-    <row r="78" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A78" s="0" t="s">
+    <row r="79" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A79" t="s">
         <v>130</v>
       </c>
     </row>
-    <row r="79" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A79" s="0" t="s">
+    <row r="80" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A80" t="s">
         <v>131</v>
       </c>
     </row>
-    <row r="80" customFormat="false" ht="32" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A80" s="0" t="s">
+    <row r="81" spans="1:4" ht="32" x14ac:dyDescent="0.2">
+      <c r="A81" t="s">
         <v>132</v>
       </c>
-      <c r="B80" s="0" t="s">
+      <c r="B81" t="s">
         <v>133</v>
       </c>
-      <c r="C80" s="0" t="s">
+      <c r="C81" t="s">
         <v>134</v>
       </c>
-      <c r="D80" s="3" t="s">
+      <c r="D81" s="3" t="s">
         <v>135</v>
       </c>
     </row>
   </sheetData>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader/>
-    <oddFooter/>
-  </headerFooter>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
+  <pageSetup paperSize="0" scale="0" firstPageNumber="0" orientation="portrait" usePrinterDefaults="0" horizontalDpi="0" verticalDpi="0" copies="0"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Added script to fit a csv table of high-P k(T)'s (from literature, for example) to Modified Arrhenius expressions
</commit_message>
<xml_diff>
--- a/Master_list.xlsx
+++ b/Master_list.xlsx
@@ -1,28 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="27610"/>
-  <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Nate/code/Work-In-Progress_scripts/"/>
-    </mc:Choice>
-  </mc:AlternateContent>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+  <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16000" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0" iterateDelta="1E-4" concurrentCalc="0"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
-      <x14:workbookPr defaultImageDpi="32767"/>
-    </ext>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
-      <mx:ArchID Flags="2"/>
-    </ext>
-  </extLst>
+  <calcPr calcId="0" iterateDelta="1E-4"/>
 </workbook>
 </file>
 
@@ -402,9 +389,6 @@
     <t>Fit_k_table_to_Chebyshev.py</t>
   </si>
   <si>
-    <t>WIP Fit_Chebyshev</t>
-  </si>
-  <si>
     <t>Zach</t>
   </si>
   <si>
@@ -440,10 +424,13 @@
 Refer to Chapter 7 of the Chemkin Input manual for instructions</t>
   </si>
   <si>
-    <t>findSpeciesInDictionary</t>
-  </si>
-  <si>
-    <t>Gives RMG name for species from an inputted RMG-dictionary from a list of SMILES</t>
+    <t>Fit_k_table_to_Modified_Arrhenius.py</t>
+  </si>
+  <si>
+    <t>WIP/Fitting_literature_k/</t>
+  </si>
+  <si>
+    <t>Fits each column of a csv table of high-P k(T) values to a Modified Arrhenius expression using Cantherm's built-in functions and outputs the fit k in Chemkin format</t>
   </si>
 </sst>
 </file>
@@ -506,7 +493,7 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium7"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <indexedColors>
       <rgbColor rgb="FF000000"/>
@@ -594,44 +581,44 @@
         <a:sysClr val="window" lastClr="FFFFFF"/>
       </a:lt1>
       <a:dk2>
-        <a:srgbClr val="44546A"/>
+        <a:srgbClr val="1F497D"/>
       </a:dk2>
       <a:lt2>
-        <a:srgbClr val="E7E6E6"/>
+        <a:srgbClr val="EEECE1"/>
       </a:lt2>
       <a:accent1>
-        <a:srgbClr val="5B9BD5"/>
+        <a:srgbClr val="4F81BD"/>
       </a:accent1>
       <a:accent2>
-        <a:srgbClr val="ED7D31"/>
+        <a:srgbClr val="C0504D"/>
       </a:accent2>
       <a:accent3>
-        <a:srgbClr val="A5A5A5"/>
+        <a:srgbClr val="9BBB59"/>
       </a:accent3>
       <a:accent4>
-        <a:srgbClr val="FFC000"/>
+        <a:srgbClr val="8064A2"/>
       </a:accent4>
       <a:accent5>
-        <a:srgbClr val="4472C4"/>
+        <a:srgbClr val="4BACC6"/>
       </a:accent5>
       <a:accent6>
-        <a:srgbClr val="70AD47"/>
+        <a:srgbClr val="F79646"/>
       </a:accent6>
       <a:hlink>
-        <a:srgbClr val="0563C1"/>
+        <a:srgbClr val="0000FF"/>
       </a:hlink>
       <a:folHlink>
-        <a:srgbClr val="954F72"/>
+        <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="Yu Gothic Light"/>
+        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
         <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="DengXian Light"/>
+        <a:font script="Hans" typeface="宋体"/>
         <a:font script="Hant" typeface="新細明體"/>
         <a:font script="Arab" typeface="Times New Roman"/>
         <a:font script="Hebr" typeface="Times New Roman"/>
@@ -661,12 +648,12 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="Yu Gothic"/>
+        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
         <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="DengXian"/>
+        <a:font script="Hans" typeface="宋体"/>
         <a:font script="Hant" typeface="新細明體"/>
         <a:font script="Arab" typeface="Arial"/>
         <a:font script="Hebr" typeface="Arial"/>
@@ -705,142 +692,166 @@
           <a:gsLst>
             <a:gs pos="0">
               <a:schemeClr val="phClr">
-                <a:lumMod val="110000"/>
-                <a:satMod val="105000"/>
-                <a:tint val="67000"/>
+                <a:tint val="50000"/>
+                <a:satMod val="300000"/>
               </a:schemeClr>
             </a:gs>
-            <a:gs pos="50000">
+            <a:gs pos="35000">
               <a:schemeClr val="phClr">
-                <a:lumMod val="105000"/>
-                <a:satMod val="103000"/>
-                <a:tint val="73000"/>
+                <a:tint val="37000"/>
+                <a:satMod val="300000"/>
               </a:schemeClr>
             </a:gs>
             <a:gs pos="100000">
               <a:schemeClr val="phClr">
-                <a:lumMod val="105000"/>
-                <a:satMod val="109000"/>
-                <a:tint val="81000"/>
+                <a:tint val="15000"/>
+                <a:satMod val="350000"/>
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin ang="5400000" scaled="0"/>
+          <a:lin ang="16200000" scaled="1"/>
         </a:gradFill>
         <a:gradFill rotWithShape="1">
           <a:gsLst>
             <a:gs pos="0">
               <a:schemeClr val="phClr">
-                <a:satMod val="103000"/>
-                <a:lumMod val="102000"/>
-                <a:tint val="94000"/>
+                <a:shade val="51000"/>
+                <a:satMod val="130000"/>
               </a:schemeClr>
             </a:gs>
-            <a:gs pos="50000">
+            <a:gs pos="80000">
               <a:schemeClr val="phClr">
-                <a:satMod val="110000"/>
-                <a:lumMod val="100000"/>
-                <a:shade val="100000"/>
+                <a:shade val="93000"/>
+                <a:satMod val="130000"/>
               </a:schemeClr>
             </a:gs>
             <a:gs pos="100000">
               <a:schemeClr val="phClr">
-                <a:lumMod val="99000"/>
-                <a:satMod val="120000"/>
-                <a:shade val="78000"/>
+                <a:shade val="94000"/>
+                <a:satMod val="135000"/>
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin ang="5400000" scaled="0"/>
+          <a:lin ang="16200000" scaled="0"/>
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
-        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr">
+              <a:shade val="95000"/>
+              <a:satMod val="105000"/>
+            </a:schemeClr>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+        </a:ln>
+        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
-          <a:miter lim="800000"/>
         </a:ln>
-        <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln w="38100" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
-          <a:miter lim="800000"/>
-        </a:ln>
-        <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
-          <a:solidFill>
-            <a:schemeClr val="phClr"/>
-          </a:solidFill>
-          <a:prstDash val="solid"/>
-          <a:miter lim="800000"/>
         </a:ln>
       </a:lnStyleLst>
       <a:effectStyleLst>
         <a:effectStyle>
-          <a:effectLst/>
-        </a:effectStyle>
-        <a:effectStyle>
-          <a:effectLst/>
+          <a:effectLst>
+            <a:outerShdw blurRad="40000" dist="20000" dir="5400000" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="38000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
               <a:srgbClr val="000000">
-                <a:alpha val="63000"/>
+                <a:alpha val="35000"/>
               </a:srgbClr>
             </a:outerShdw>
           </a:effectLst>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst>
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="35000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
+          <a:scene3d>
+            <a:camera prst="orthographicFront">
+              <a:rot lat="0" lon="0" rev="0"/>
+            </a:camera>
+            <a:lightRig rig="threePt" dir="t">
+              <a:rot lat="0" lon="0" rev="1200000"/>
+            </a:lightRig>
+          </a:scene3d>
+          <a:sp3d>
+            <a:bevelT w="63500" h="25400"/>
+          </a:sp3d>
         </a:effectStyle>
       </a:effectStyleLst>
       <a:bgFillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
         </a:solidFill>
-        <a:solidFill>
-          <a:schemeClr val="phClr">
-            <a:tint val="95000"/>
-            <a:satMod val="170000"/>
-          </a:schemeClr>
-        </a:solidFill>
         <a:gradFill rotWithShape="1">
           <a:gsLst>
             <a:gs pos="0">
               <a:schemeClr val="phClr">
-                <a:tint val="93000"/>
-                <a:satMod val="150000"/>
-                <a:shade val="98000"/>
-                <a:lumMod val="102000"/>
+                <a:tint val="40000"/>
+                <a:satMod val="350000"/>
               </a:schemeClr>
             </a:gs>
-            <a:gs pos="50000">
+            <a:gs pos="40000">
               <a:schemeClr val="phClr">
-                <a:tint val="98000"/>
-                <a:satMod val="130000"/>
-                <a:shade val="90000"/>
-                <a:lumMod val="103000"/>
+                <a:tint val="45000"/>
+                <a:shade val="99000"/>
+                <a:satMod val="350000"/>
               </a:schemeClr>
             </a:gs>
             <a:gs pos="100000">
               <a:schemeClr val="phClr">
-                <a:shade val="63000"/>
-                <a:satMod val="120000"/>
+                <a:shade val="20000"/>
+                <a:satMod val="255000"/>
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin ang="5400000" scaled="0"/>
+          <a:path path="circle">
+            <a:fillToRect l="50000" t="-80000" r="50000" b="180000"/>
+          </a:path>
+        </a:gradFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:tint val="80000"/>
+                <a:satMod val="300000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:shade val="30000"/>
+                <a:satMod val="200000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:path path="circle">
+            <a:fillToRect l="50000" t="50000" r="50000" b="50000"/>
+          </a:path>
         </a:gradFill>
       </a:bgFillStyleLst>
     </a:fmtScheme>
   </a:themeElements>
   <a:objectDefaults/>
   <a:extraClrSchemeLst/>
-  <a:extLst>
-    <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
-    </a:ext>
-  </a:extLst>
 </a:theme>
 </file>
 
@@ -848,22 +859,25 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D81"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D22" sqref="D22"/>
+    <sheetView tabSelected="1" topLeftCell="A50" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B73" sqref="B73"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="66.1640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="109.1640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="67"/>
+    <col min="2" max="2" width="66.875"/>
+    <col min="3" max="3" width="31.5"/>
+    <col min="4" max="4" width="100.5"/>
+    <col min="5" max="1025" width="11"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" s="2" customFormat="1" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:4" s="2" customFormat="1" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
@@ -877,7 +891,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>5</v>
       </c>
@@ -891,7 +905,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>9</v>
       </c>
@@ -905,7 +919,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>11</v>
       </c>
@@ -919,7 +933,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>13</v>
       </c>
@@ -933,7 +947,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>15</v>
       </c>
@@ -947,7 +961,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>19</v>
       </c>
@@ -961,12 +975,12 @@
         <v>20</v>
       </c>
     </row>
-    <row r="10" spans="1:4" s="2" customFormat="1" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:4" s="2" customFormat="1" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="11" spans="1:4" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:4" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
         <v>1</v>
       </c>
@@ -980,7 +994,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>22</v>
       </c>
@@ -991,7 +1005,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>25</v>
       </c>
@@ -1005,7 +1019,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>27</v>
       </c>
@@ -1016,7 +1030,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>29</v>
       </c>
@@ -1030,7 +1044,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>32</v>
       </c>
@@ -1044,7 +1058,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>34</v>
       </c>
@@ -1058,7 +1072,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>36</v>
       </c>
@@ -1072,7 +1086,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>38</v>
       </c>
@@ -1086,12 +1100,12 @@
         <v>39</v>
       </c>
     </row>
-    <row r="21" spans="1:4" s="2" customFormat="1" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:4" s="2" customFormat="1" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="22" spans="1:4" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:4" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="2" t="s">
         <v>1</v>
       </c>
@@ -1105,7 +1119,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>41</v>
       </c>
@@ -1119,7 +1133,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>44</v>
       </c>
@@ -1133,139 +1147,139 @@
         <v>46</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A25" t="s">
-        <v>136</v>
-      </c>
-      <c r="B25" t="s">
+    <row r="26" spans="1:4" s="2" customFormat="1" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A26" s="1" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A27" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B27" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C27" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="D27" s="2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>48</v>
+      </c>
+      <c r="B28" t="s">
+        <v>49</v>
+      </c>
+      <c r="C28" t="s">
+        <v>50</v>
+      </c>
+      <c r="D28" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>52</v>
+      </c>
+      <c r="B29" t="s">
+        <v>23</v>
+      </c>
+      <c r="C29" t="s">
+        <v>53</v>
+      </c>
+      <c r="D29" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>55</v>
+      </c>
+      <c r="B30" t="s">
         <v>56</v>
       </c>
-      <c r="C25" t="s">
+      <c r="C30" t="s">
         <v>17</v>
       </c>
-      <c r="D25" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="27" spans="1:4" s="2" customFormat="1" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A27" s="1" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="28" spans="1:4" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A28" s="2" t="s">
+      <c r="D30" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>58</v>
+      </c>
+      <c r="B31" t="s">
+        <v>59</v>
+      </c>
+      <c r="C31" t="s">
+        <v>60</v>
+      </c>
+      <c r="D31" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>62</v>
+      </c>
+      <c r="B32" t="s">
+        <v>63</v>
+      </c>
+      <c r="D32" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>65</v>
+      </c>
+      <c r="B33" t="s">
+        <v>66</v>
+      </c>
+      <c r="D33" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" s="2" customFormat="1" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A35" s="1" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A36" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B28" s="2" t="s">
+      <c r="B36" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="C28" s="2" t="s">
+      <c r="C36" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="D28" s="2" t="s">
+      <c r="D36" s="2" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A29" t="s">
-        <v>48</v>
-      </c>
-      <c r="B29" t="s">
-        <v>49</v>
-      </c>
-      <c r="C29" t="s">
-        <v>50</v>
-      </c>
-      <c r="D29" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A30" t="s">
-        <v>52</v>
-      </c>
-      <c r="B30" t="s">
-        <v>23</v>
-      </c>
-      <c r="C30" t="s">
-        <v>53</v>
-      </c>
-      <c r="D30" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A31" t="s">
-        <v>55</v>
-      </c>
-      <c r="B31" t="s">
-        <v>56</v>
-      </c>
-      <c r="C31" t="s">
-        <v>17</v>
-      </c>
-      <c r="D31" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A32" t="s">
-        <v>58</v>
-      </c>
-      <c r="B32" t="s">
-        <v>59</v>
-      </c>
-      <c r="C32" t="s">
-        <v>60</v>
-      </c>
-      <c r="D32" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A33" t="s">
-        <v>62</v>
-      </c>
-      <c r="B33" t="s">
-        <v>63</v>
-      </c>
-      <c r="D33" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A34" t="s">
-        <v>65</v>
-      </c>
-      <c r="B34" t="s">
-        <v>66</v>
-      </c>
-      <c r="D34" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="36" spans="1:4" s="2" customFormat="1" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A36" s="1" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="37" spans="1:4" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A37" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="B37" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="C37" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="D37" s="2" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
+        <v>69</v>
+      </c>
+      <c r="B37" t="s">
+        <v>6</v>
+      </c>
+      <c r="C37" t="s">
+        <v>7</v>
+      </c>
+      <c r="D37" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>69</v>
+        <v>5</v>
       </c>
       <c r="B38" t="s">
         <v>6</v>
@@ -1274,153 +1288,153 @@
         <v>7</v>
       </c>
       <c r="D38" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.2">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>5</v>
+        <v>72</v>
       </c>
       <c r="B39" t="s">
-        <v>6</v>
-      </c>
-      <c r="C39" t="s">
-        <v>7</v>
+        <v>63</v>
       </c>
       <c r="D39" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.2">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="B40" t="s">
         <v>63</v>
       </c>
       <c r="D40" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.2">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="B41" t="s">
-        <v>63</v>
+        <v>56</v>
+      </c>
+      <c r="C41" t="s">
+        <v>7</v>
       </c>
       <c r="D41" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A42" t="s">
-        <v>76</v>
-      </c>
-      <c r="B42" t="s">
-        <v>56</v>
-      </c>
-      <c r="C42" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" s="2" customFormat="1" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A43" s="1" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A44" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B44" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C44" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="D44" s="2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A45" t="s">
+        <v>79</v>
+      </c>
+      <c r="B45" t="s">
+        <v>30</v>
+      </c>
+      <c r="C45" t="s">
         <v>7</v>
       </c>
-      <c r="D42" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="44" spans="1:4" s="2" customFormat="1" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A44" s="1" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="45" spans="1:4" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A45" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="B45" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="C45" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="D45" s="2" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="D45" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="B46" t="s">
         <v>30</v>
       </c>
       <c r="C46" t="s">
-        <v>7</v>
+        <v>17</v>
       </c>
       <c r="D46" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.2">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="B47" t="s">
-        <v>30</v>
+        <v>84</v>
       </c>
       <c r="C47" t="s">
+        <v>85</v>
+      </c>
+      <c r="D47" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4" s="2" customFormat="1" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A49" s="1" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="50" spans="1:4" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A50" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B50" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C50" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="D50" s="2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A51" t="s">
+        <v>88</v>
+      </c>
+      <c r="B51" t="s">
+        <v>89</v>
+      </c>
+      <c r="D51" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A52" t="s">
+        <v>91</v>
+      </c>
+      <c r="B52" t="s">
+        <v>92</v>
+      </c>
+      <c r="C52" t="s">
         <v>17</v>
       </c>
-      <c r="D47" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A48" t="s">
-        <v>83</v>
-      </c>
-      <c r="B48" t="s">
-        <v>84</v>
-      </c>
-      <c r="C48" t="s">
-        <v>85</v>
-      </c>
-      <c r="D48" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="50" spans="1:4" s="2" customFormat="1" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A50" s="1" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="51" spans="1:4" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A51" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="B51" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="C51" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="D51" s="2" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A52" t="s">
-        <v>88</v>
-      </c>
-      <c r="B52" t="s">
-        <v>89</v>
-      </c>
       <c r="D52" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.2">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>91</v>
+        <v>94</v>
       </c>
       <c r="B53" t="s">
         <v>92</v>
@@ -1429,45 +1443,45 @@
         <v>17</v>
       </c>
       <c r="D53" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A54" t="s">
-        <v>94</v>
-      </c>
-      <c r="B54" t="s">
-        <v>92</v>
-      </c>
-      <c r="C54" t="s">
-        <v>17</v>
-      </c>
-      <c r="D54" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="56" spans="1:4" s="2" customFormat="1" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A56" s="1" t="s">
+    <row r="55" spans="1:4" s="2" customFormat="1" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A55" s="1" t="s">
         <v>96</v>
       </c>
     </row>
-    <row r="57" spans="1:4" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A57" s="2" t="s">
+    <row r="56" spans="1:4" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A56" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B57" s="2" t="s">
+      <c r="B56" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="C57" s="2" t="s">
+      <c r="C56" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="D57" s="2" t="s">
+      <c r="D56" s="2" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="58" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A58" s="4" t="s">
+    <row r="57" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A57" s="4" t="s">
         <v>97</v>
+      </c>
+      <c r="B57" t="s">
+        <v>6</v>
+      </c>
+      <c r="C57" t="s">
+        <v>7</v>
+      </c>
+      <c r="D57" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="58" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A58" t="s">
+        <v>99</v>
       </c>
       <c r="B58" t="s">
         <v>6</v>
@@ -1476,170 +1490,170 @@
         <v>7</v>
       </c>
       <c r="D58" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="59" spans="1:4" x14ac:dyDescent="0.2">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="59" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
       <c r="B59" t="s">
+        <v>102</v>
+      </c>
+      <c r="D59" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="60" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A60" t="s">
+        <v>104</v>
+      </c>
+      <c r="B60" t="s">
+        <v>23</v>
+      </c>
+      <c r="D60" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="61" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A61" t="s">
+        <v>106</v>
+      </c>
+      <c r="B61" t="s">
+        <v>107</v>
+      </c>
+      <c r="C61" t="s">
+        <v>17</v>
+      </c>
+      <c r="D61" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="62" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A62" t="s">
+        <v>109</v>
+      </c>
+      <c r="B62" t="s">
         <v>6</v>
       </c>
-      <c r="C59" t="s">
+      <c r="C62" t="s">
         <v>7</v>
       </c>
-      <c r="D59" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="60" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A60" t="s">
-        <v>101</v>
-      </c>
-      <c r="B60" t="s">
-        <v>102</v>
-      </c>
-      <c r="D60" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="61" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A61" t="s">
-        <v>104</v>
-      </c>
-      <c r="B61" t="s">
-        <v>23</v>
-      </c>
-      <c r="D61" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="62" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A62" t="s">
-        <v>106</v>
-      </c>
-      <c r="B62" t="s">
-        <v>107</v>
-      </c>
-      <c r="C62" t="s">
-        <v>17</v>
-      </c>
       <c r="D62" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="63" spans="1:4" x14ac:dyDescent="0.2">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="63" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
-        <v>109</v>
+        <v>111</v>
       </c>
       <c r="B63" t="s">
-        <v>6</v>
+        <v>112</v>
       </c>
       <c r="C63" t="s">
-        <v>7</v>
+        <v>53</v>
       </c>
       <c r="D63" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="64" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A64" t="s">
-        <v>111</v>
-      </c>
-      <c r="B64" t="s">
-        <v>112</v>
-      </c>
-      <c r="C64" t="s">
-        <v>53</v>
-      </c>
-      <c r="D64" t="s">
         <v>113</v>
       </c>
     </row>
-    <row r="66" spans="1:4" s="2" customFormat="1" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A66" s="1" t="s">
+    <row r="65" spans="1:4" s="2" customFormat="1" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A65" s="1" t="s">
         <v>114</v>
       </c>
     </row>
-    <row r="67" spans="1:4" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A67" s="2" t="s">
+    <row r="66" spans="1:4" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A66" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B67" s="2" t="s">
+      <c r="B66" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="C67" s="2" t="s">
+      <c r="C66" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="D67" s="2" t="s">
+      <c r="D66" s="2" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="68" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A67" t="s">
+        <v>115</v>
+      </c>
+      <c r="B67" t="s">
+        <v>116</v>
+      </c>
+      <c r="C67" t="s">
+        <v>117</v>
+      </c>
+      <c r="D67" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="68" spans="1:4" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
-        <v>115</v>
+        <v>119</v>
       </c>
       <c r="B68" t="s">
-        <v>116</v>
-      </c>
-      <c r="C68" t="s">
-        <v>117</v>
-      </c>
-      <c r="D68" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="69" spans="1:4" ht="32" x14ac:dyDescent="0.2">
-      <c r="A69" t="s">
-        <v>119</v>
-      </c>
-      <c r="B69" t="s">
         <v>120</v>
       </c>
-      <c r="D69" s="3" t="s">
+      <c r="D68" s="3" t="s">
         <v>121</v>
       </c>
     </row>
-    <row r="71" spans="1:4" s="2" customFormat="1" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A71" s="1" t="s">
+    <row r="70" spans="1:4" s="2" customFormat="1" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A70" s="1" t="s">
         <v>122</v>
       </c>
     </row>
-    <row r="72" spans="1:4" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A72" s="2" t="s">
+    <row r="71" spans="1:4" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A71" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B72" s="2" t="s">
+      <c r="B71" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="C72" s="2" t="s">
+      <c r="C71" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="D72" s="2" t="s">
+      <c r="D71" s="2" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="73" spans="1:4" ht="32" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:4" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A72" t="s">
+        <v>123</v>
+      </c>
+      <c r="B72" t="s">
+        <v>136</v>
+      </c>
+      <c r="C72" t="s">
+        <v>124</v>
+      </c>
+      <c r="D72" s="3" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="73" spans="1:4" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
-        <v>123</v>
+        <v>135</v>
       </c>
       <c r="B73" t="s">
+        <v>136</v>
+      </c>
+      <c r="C73" t="s">
         <v>124</v>
       </c>
-      <c r="C73" t="s">
-        <v>125</v>
-      </c>
       <c r="D73" s="3" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="75" spans="1:4" s="2" customFormat="1" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A75" s="1" t="s">
         <v>126</v>
       </c>
     </row>
-    <row r="75" spans="1:4" s="2" customFormat="1" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A75" s="1" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="76" spans="1:4" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:4" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A76" s="2" t="s">
         <v>1</v>
       </c>
@@ -1653,38 +1667,38 @@
         <v>4</v>
       </c>
     </row>
-    <row r="77" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="77" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="78" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A78" t="s">
         <v>128</v>
       </c>
     </row>
-    <row r="78" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A78" t="s">
+    <row r="79" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A79" t="s">
         <v>129</v>
       </c>
     </row>
-    <row r="79" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A79" t="s">
+    <row r="80" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A80" t="s">
         <v>130</v>
       </c>
     </row>
-    <row r="80" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A80" t="s">
+    <row r="81" spans="1:4" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A81" t="s">
         <v>131</v>
       </c>
-    </row>
-    <row r="81" spans="1:4" ht="32" x14ac:dyDescent="0.2">
-      <c r="A81" t="s">
+      <c r="B81" t="s">
         <v>132</v>
       </c>
-      <c r="B81" t="s">
+      <c r="C81" t="s">
         <v>133</v>
       </c>
-      <c r="C81" t="s">
+      <c r="D81" s="3" t="s">
         <v>134</v>
-      </c>
-      <c r="D81" s="3" t="s">
-        <v>135</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add plotRxnPathDiagram info into the Master_list.xlsx.
</commit_message>
<xml_diff>
--- a/Master_list.xlsx
+++ b/Master_list.xlsx
@@ -1,10 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\RMG\Work-In-Progress_scripts\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8196" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -14,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="229" uniqueCount="138">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="233" uniqueCount="142">
   <si>
     <t>Quick operations for one data point</t>
   </si>
@@ -431,6 +436,18 @@
   </si>
   <si>
     <t>Fits each column of a csv table of high-P k(T) values to a Modified Arrhenius expression using Cantherm's built-in functions and outputs the fit k in Chemkin format</t>
+  </si>
+  <si>
+    <t>plotRxnPathDiagram</t>
+  </si>
+  <si>
+    <t>WIP/model_analyzer/plotRxnPathDiagram</t>
+  </si>
+  <si>
+    <t>Peng</t>
+  </si>
+  <si>
+    <t>Plot rxn path diagram for constant V simulation using Cantera. The nodes in the output diagram is labeled with species images.</t>
   </si>
 </sst>
 </file>
@@ -566,6 +583,9 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
     </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
   </extLst>
 </styleSheet>
 </file>
@@ -613,7 +633,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -648,7 +668,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -857,27 +877,27 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D81"/>
+  <dimension ref="A1:D82"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A50" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B73" sqref="B73"/>
+      <selection activeCell="D64" sqref="D64"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="67"/>
-    <col min="2" max="2" width="66.875"/>
+    <col min="2" max="2" width="66.8984375"/>
     <col min="3" max="3" width="31.5"/>
     <col min="4" max="4" width="100.5"/>
     <col min="5" max="1025" width="11"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" s="2" customFormat="1" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" s="2" customFormat="1" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
@@ -891,7 +911,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>5</v>
       </c>
@@ -905,7 +925,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>9</v>
       </c>
@@ -919,7 +939,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>11</v>
       </c>
@@ -933,7 +953,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>13</v>
       </c>
@@ -947,7 +967,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>15</v>
       </c>
@@ -961,7 +981,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>19</v>
       </c>
@@ -975,12 +995,12 @@
         <v>20</v>
       </c>
     </row>
-    <row r="10" spans="1:4" s="2" customFormat="1" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:4" s="2" customFormat="1" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="11" spans="1:4" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:4" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="2" t="s">
         <v>1</v>
       </c>
@@ -994,7 +1014,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>22</v>
       </c>
@@ -1005,7 +1025,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>25</v>
       </c>
@@ -1019,7 +1039,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>27</v>
       </c>
@@ -1030,7 +1050,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>29</v>
       </c>
@@ -1044,7 +1064,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>32</v>
       </c>
@@ -1058,7 +1078,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>34</v>
       </c>
@@ -1072,7 +1092,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>36</v>
       </c>
@@ -1086,7 +1106,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>38</v>
       </c>
@@ -1100,12 +1120,12 @@
         <v>39</v>
       </c>
     </row>
-    <row r="21" spans="1:4" s="2" customFormat="1" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:4" s="2" customFormat="1" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A21" s="1" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="22" spans="1:4" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:4" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A22" s="2" t="s">
         <v>1</v>
       </c>
@@ -1119,7 +1139,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>41</v>
       </c>
@@ -1133,7 +1153,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>44</v>
       </c>
@@ -1147,12 +1167,12 @@
         <v>46</v>
       </c>
     </row>
-    <row r="26" spans="1:4" s="2" customFormat="1" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:4" s="2" customFormat="1" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A26" s="1" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="27" spans="1:4" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:4" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A27" s="2" t="s">
         <v>1</v>
       </c>
@@ -1166,7 +1186,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>48</v>
       </c>
@@ -1180,7 +1200,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
         <v>52</v>
       </c>
@@ -1194,7 +1214,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
         <v>55</v>
       </c>
@@ -1208,7 +1228,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
         <v>58</v>
       </c>
@@ -1222,7 +1242,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
         <v>62</v>
       </c>
@@ -1233,7 +1253,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
         <v>65</v>
       </c>
@@ -1244,12 +1264,12 @@
         <v>67</v>
       </c>
     </row>
-    <row r="35" spans="1:4" s="2" customFormat="1" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:4" s="2" customFormat="1" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A35" s="1" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="36" spans="1:4" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:4" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A36" s="2" t="s">
         <v>1</v>
       </c>
@@ -1263,7 +1283,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
         <v>69</v>
       </c>
@@ -1277,7 +1297,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
         <v>5</v>
       </c>
@@ -1291,7 +1311,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
         <v>72</v>
       </c>
@@ -1302,7 +1322,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
         <v>74</v>
       </c>
@@ -1313,7 +1333,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
         <v>76</v>
       </c>
@@ -1327,12 +1347,12 @@
         <v>77</v>
       </c>
     </row>
-    <row r="43" spans="1:4" s="2" customFormat="1" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:4" s="2" customFormat="1" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A43" s="1" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="44" spans="1:4" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:4" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A44" s="2" t="s">
         <v>1</v>
       </c>
@@ -1346,7 +1366,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
         <v>79</v>
       </c>
@@ -1360,7 +1380,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
         <v>81</v>
       </c>
@@ -1374,7 +1394,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
         <v>83</v>
       </c>
@@ -1388,12 +1408,12 @@
         <v>86</v>
       </c>
     </row>
-    <row r="49" spans="1:4" s="2" customFormat="1" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:4" s="2" customFormat="1" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A49" s="1" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="50" spans="1:4" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:4" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A50" s="2" t="s">
         <v>1</v>
       </c>
@@ -1407,7 +1427,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
         <v>88</v>
       </c>
@@ -1418,7 +1438,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
         <v>91</v>
       </c>
@@ -1432,7 +1452,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
         <v>94</v>
       </c>
@@ -1446,12 +1466,12 @@
         <v>95</v>
       </c>
     </row>
-    <row r="55" spans="1:4" s="2" customFormat="1" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:4" s="2" customFormat="1" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A55" s="1" t="s">
         <v>96</v>
       </c>
     </row>
-    <row r="56" spans="1:4" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:4" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A56" s="2" t="s">
         <v>1</v>
       </c>
@@ -1465,7 +1485,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="57" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A57" s="4" t="s">
         <v>97</v>
       </c>
@@ -1479,7 +1499,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="58" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A58" t="s">
         <v>99</v>
       </c>
@@ -1493,7 +1513,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="59" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A59" t="s">
         <v>101</v>
       </c>
@@ -1504,7 +1524,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="60" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A60" t="s">
         <v>104</v>
       </c>
@@ -1515,7 +1535,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="61" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A61" t="s">
         <v>106</v>
       </c>
@@ -1529,7 +1549,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="62" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A62" t="s">
         <v>109</v>
       </c>
@@ -1543,7 +1563,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="63" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A63" t="s">
         <v>111</v>
       </c>
@@ -1557,86 +1577,86 @@
         <v>113</v>
       </c>
     </row>
-    <row r="65" spans="1:4" s="2" customFormat="1" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A65" s="1" t="s">
+    <row r="64" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A64" t="s">
+        <v>138</v>
+      </c>
+      <c r="B64" t="s">
+        <v>139</v>
+      </c>
+      <c r="C64" t="s">
+        <v>140</v>
+      </c>
+      <c r="D64" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="66" spans="1:4" s="2" customFormat="1" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A66" s="1" t="s">
         <v>114</v>
       </c>
     </row>
-    <row r="66" spans="1:4" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A66" s="2" t="s">
+    <row r="67" spans="1:4" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A67" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B66" s="2" t="s">
+      <c r="B67" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="C66" s="2" t="s">
+      <c r="C67" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="D66" s="2" t="s">
+      <c r="D67" s="2" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="67" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A67" t="s">
+    <row r="68" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A68" t="s">
         <v>115</v>
       </c>
-      <c r="B67" t="s">
+      <c r="B68" t="s">
         <v>116</v>
       </c>
-      <c r="C67" t="s">
+      <c r="C68" t="s">
         <v>117</v>
       </c>
-      <c r="D67" t="s">
+      <c r="D68" t="s">
         <v>118</v>
       </c>
     </row>
-    <row r="68" spans="1:4" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A68" t="s">
+    <row r="69" spans="1:4" ht="31.2" x14ac:dyDescent="0.3">
+      <c r="A69" t="s">
         <v>119</v>
       </c>
-      <c r="B68" t="s">
+      <c r="B69" t="s">
         <v>120</v>
       </c>
-      <c r="D68" s="3" t="s">
+      <c r="D69" s="3" t="s">
         <v>121</v>
       </c>
     </row>
-    <row r="70" spans="1:4" s="2" customFormat="1" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A70" s="1" t="s">
+    <row r="71" spans="1:4" s="2" customFormat="1" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A71" s="1" t="s">
         <v>122</v>
       </c>
     </row>
-    <row r="71" spans="1:4" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A71" s="2" t="s">
+    <row r="72" spans="1:4" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A72" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B71" s="2" t="s">
+      <c r="B72" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="C71" s="2" t="s">
+      <c r="C72" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="D71" s="2" t="s">
+      <c r="D72" s="2" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="72" spans="1:4" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A72" t="s">
+    <row r="73" spans="1:4" ht="46.8" x14ac:dyDescent="0.3">
+      <c r="A73" t="s">
         <v>123</v>
-      </c>
-      <c r="B72" t="s">
-        <v>136</v>
-      </c>
-      <c r="C72" t="s">
-        <v>124</v>
-      </c>
-      <c r="D72" s="3" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="73" spans="1:4" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A73" t="s">
-        <v>135</v>
       </c>
       <c r="B73" t="s">
         <v>136</v>
@@ -1645,59 +1665,73 @@
         <v>124</v>
       </c>
       <c r="D73" s="3" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="74" spans="1:4" ht="31.2" x14ac:dyDescent="0.3">
+      <c r="A74" t="s">
+        <v>135</v>
+      </c>
+      <c r="B74" t="s">
+        <v>136</v>
+      </c>
+      <c r="C74" t="s">
+        <v>124</v>
+      </c>
+      <c r="D74" s="3" t="s">
         <v>137</v>
       </c>
     </row>
-    <row r="75" spans="1:4" s="2" customFormat="1" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A75" s="1" t="s">
+    <row r="76" spans="1:4" s="2" customFormat="1" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A76" s="1" t="s">
         <v>126</v>
       </c>
     </row>
-    <row r="76" spans="1:4" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A76" s="2" t="s">
+    <row r="77" spans="1:4" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A77" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B76" s="2" t="s">
+      <c r="B77" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="C76" s="2" t="s">
+      <c r="C77" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="D76" s="2" t="s">
+      <c r="D77" s="2" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="77" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A77" t="s">
+    <row r="78" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A78" t="s">
         <v>127</v>
       </c>
     </row>
-    <row r="78" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A78" t="s">
+    <row r="79" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A79" t="s">
         <v>128</v>
       </c>
     </row>
-    <row r="79" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A79" t="s">
+    <row r="80" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A80" t="s">
         <v>129</v>
       </c>
     </row>
-    <row r="80" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A80" t="s">
+    <row r="81" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A81" t="s">
         <v>130</v>
       </c>
     </row>
-    <row r="81" spans="1:4" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A81" t="s">
+    <row r="82" spans="1:4" ht="31.2" x14ac:dyDescent="0.3">
+      <c r="A82" t="s">
         <v>131</v>
       </c>
-      <c r="B81" t="s">
+      <c r="B82" t="s">
         <v>132</v>
       </c>
-      <c r="C81" t="s">
+      <c r="C82" t="s">
         <v>133</v>
       </c>
-      <c r="D81" s="3" t="s">
+      <c r="D82" s="3" t="s">
         <v>134</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Added script to convert a species dictionary to all Kekulized bonds for aromatic species
</commit_message>
<xml_diff>
--- a/Master_list.xlsx
+++ b/Master_list.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="229" uniqueCount="138">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="233" uniqueCount="140">
   <si>
     <t>Quick operations for one data point</t>
   </si>
@@ -431,6 +431,12 @@
   </si>
   <si>
     <t>Fits each column of a csv table of high-P k(T) values to a Modified Arrhenius expression using Cantherm's built-in functions and outputs the fit k in Chemkin format</t>
+  </si>
+  <si>
+    <t>dictionaryToKekulized.py</t>
+  </si>
+  <si>
+    <t>For an existing species dictionary, convert adjacency lists for aromatic species to kekulized bond types</t>
   </si>
 </sst>
 </file>
@@ -857,10 +863,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D81"/>
+  <dimension ref="A1:D82"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A50" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B73" sqref="B73"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A17" sqref="A17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -1100,186 +1106,186 @@
         <v>39</v>
       </c>
     </row>
-    <row r="21" spans="1:4" s="2" customFormat="1" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="1" t="s">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>138</v>
+      </c>
+      <c r="B20" t="s">
+        <v>30</v>
+      </c>
+      <c r="C20" t="s">
+        <v>7</v>
+      </c>
+      <c r="D20" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" s="2" customFormat="1" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A22" s="1" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="22" spans="1:4" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="2" t="s">
+    <row r="23" spans="1:4" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A23" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B22" s="2" t="s">
+      <c r="B23" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="C22" s="2" t="s">
+      <c r="C23" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="D22" s="2" t="s">
+      <c r="D23" s="2" t="s">
         <v>4</v>
-      </c>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A23" t="s">
-        <v>41</v>
-      </c>
-      <c r="B23" t="s">
-        <v>42</v>
-      </c>
-      <c r="C23" t="s">
-        <v>17</v>
-      </c>
-      <c r="D23" t="s">
-        <v>43</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="B24" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="C24" t="s">
         <v>17</v>
       </c>
       <c r="D24" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>44</v>
+      </c>
+      <c r="B25" t="s">
+        <v>45</v>
+      </c>
+      <c r="C25" t="s">
+        <v>17</v>
+      </c>
+      <c r="D25" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="26" spans="1:4" s="2" customFormat="1" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="1" t="s">
+    <row r="27" spans="1:4" s="2" customFormat="1" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A27" s="1" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="27" spans="1:4" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="2" t="s">
+    <row r="28" spans="1:4" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A28" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B27" s="2" t="s">
+      <c r="B28" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="C27" s="2" t="s">
+      <c r="C28" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="D27" s="2" t="s">
+      <c r="D28" s="2" t="s">
         <v>4</v>
-      </c>
-    </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A28" t="s">
-        <v>48</v>
-      </c>
-      <c r="B28" t="s">
-        <v>49</v>
-      </c>
-      <c r="C28" t="s">
-        <v>50</v>
-      </c>
-      <c r="D28" t="s">
-        <v>51</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="B29" t="s">
-        <v>23</v>
+        <v>49</v>
       </c>
       <c r="C29" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="D29" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="B30" t="s">
-        <v>56</v>
+        <v>23</v>
       </c>
       <c r="C30" t="s">
-        <v>17</v>
+        <v>53</v>
       </c>
       <c r="D30" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="B31" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="C31" t="s">
-        <v>60</v>
+        <v>17</v>
       </c>
       <c r="D31" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="B32" t="s">
-        <v>63</v>
+        <v>59</v>
+      </c>
+      <c r="C32" t="s">
+        <v>60</v>
       </c>
       <c r="D32" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
+        <v>62</v>
+      </c>
+      <c r="B33" t="s">
+        <v>63</v>
+      </c>
+      <c r="D33" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
         <v>65</v>
       </c>
-      <c r="B33" t="s">
+      <c r="B34" t="s">
         <v>66</v>
       </c>
-      <c r="D33" t="s">
+      <c r="D34" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="35" spans="1:4" s="2" customFormat="1" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A35" s="1" t="s">
+    <row r="36" spans="1:4" s="2" customFormat="1" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A36" s="1" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="36" spans="1:4" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A36" s="2" t="s">
+    <row r="37" spans="1:4" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A37" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B36" s="2" t="s">
+      <c r="B37" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="C36" s="2" t="s">
+      <c r="C37" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="D36" s="2" t="s">
+      <c r="D37" s="2" t="s">
         <v>4</v>
-      </c>
-    </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A37" t="s">
-        <v>69</v>
-      </c>
-      <c r="B37" t="s">
-        <v>6</v>
-      </c>
-      <c r="C37" t="s">
-        <v>7</v>
-      </c>
-      <c r="D37" t="s">
-        <v>70</v>
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>5</v>
+        <v>69</v>
       </c>
       <c r="B38" t="s">
         <v>6</v>
@@ -1288,153 +1294,153 @@
         <v>7</v>
       </c>
       <c r="D38" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>72</v>
+        <v>5</v>
       </c>
       <c r="B39" t="s">
-        <v>63</v>
+        <v>6</v>
+      </c>
+      <c r="C39" t="s">
+        <v>7</v>
       </c>
       <c r="D39" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="B40" t="s">
         <v>63</v>
       </c>
       <c r="D40" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
+        <v>74</v>
+      </c>
+      <c r="B41" t="s">
+        <v>63</v>
+      </c>
+      <c r="D41" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A42" t="s">
         <v>76</v>
       </c>
-      <c r="B41" t="s">
+      <c r="B42" t="s">
         <v>56</v>
       </c>
-      <c r="C41" t="s">
+      <c r="C42" t="s">
         <v>7</v>
       </c>
-      <c r="D41" t="s">
+      <c r="D42" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="43" spans="1:4" s="2" customFormat="1" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A43" s="1" t="s">
+    <row r="44" spans="1:4" s="2" customFormat="1" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A44" s="1" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="44" spans="1:4" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A44" s="2" t="s">
+    <row r="45" spans="1:4" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A45" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B44" s="2" t="s">
+      <c r="B45" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="C44" s="2" t="s">
+      <c r="C45" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="D44" s="2" t="s">
+      <c r="D45" s="2" t="s">
         <v>4</v>
-      </c>
-    </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A45" t="s">
-        <v>79</v>
-      </c>
-      <c r="B45" t="s">
-        <v>30</v>
-      </c>
-      <c r="C45" t="s">
-        <v>7</v>
-      </c>
-      <c r="D45" t="s">
-        <v>80</v>
       </c>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="B46" t="s">
         <v>30</v>
       </c>
       <c r="C46" t="s">
-        <v>17</v>
+        <v>7</v>
       </c>
       <c r="D46" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
+        <v>81</v>
+      </c>
+      <c r="B47" t="s">
+        <v>30</v>
+      </c>
+      <c r="C47" t="s">
+        <v>17</v>
+      </c>
+      <c r="D47" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A48" t="s">
         <v>83</v>
       </c>
-      <c r="B47" t="s">
+      <c r="B48" t="s">
         <v>84</v>
       </c>
-      <c r="C47" t="s">
+      <c r="C48" t="s">
         <v>85</v>
       </c>
-      <c r="D47" t="s">
+      <c r="D48" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="49" spans="1:4" s="2" customFormat="1" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A49" s="1" t="s">
+    <row r="50" spans="1:4" s="2" customFormat="1" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A50" s="1" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="50" spans="1:4" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A50" s="2" t="s">
+    <row r="51" spans="1:4" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A51" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B50" s="2" t="s">
+      <c r="B51" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="C50" s="2" t="s">
+      <c r="C51" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="D50" s="2" t="s">
+      <c r="D51" s="2" t="s">
         <v>4</v>
-      </c>
-    </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A51" t="s">
-        <v>88</v>
-      </c>
-      <c r="B51" t="s">
-        <v>89</v>
-      </c>
-      <c r="D51" t="s">
-        <v>90</v>
       </c>
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="B52" t="s">
-        <v>92</v>
-      </c>
-      <c r="C52" t="s">
-        <v>17</v>
+        <v>89</v>
       </c>
       <c r="D52" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="B53" t="s">
         <v>92</v>
@@ -1443,45 +1449,45 @@
         <v>17</v>
       </c>
       <c r="D53" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A54" t="s">
+        <v>94</v>
+      </c>
+      <c r="B54" t="s">
+        <v>92</v>
+      </c>
+      <c r="C54" t="s">
+        <v>17</v>
+      </c>
+      <c r="D54" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="55" spans="1:4" s="2" customFormat="1" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A55" s="1" t="s">
+    <row r="56" spans="1:4" s="2" customFormat="1" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A56" s="1" t="s">
         <v>96</v>
       </c>
     </row>
-    <row r="56" spans="1:4" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A56" s="2" t="s">
+    <row r="57" spans="1:4" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A57" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B56" s="2" t="s">
+      <c r="B57" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="C56" s="2" t="s">
+      <c r="C57" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="D56" s="2" t="s">
+      <c r="D57" s="2" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="57" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A57" s="4" t="s">
+    <row r="58" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A58" s="4" t="s">
         <v>97</v>
-      </c>
-      <c r="B57" t="s">
-        <v>6</v>
-      </c>
-      <c r="C57" t="s">
-        <v>7</v>
-      </c>
-      <c r="D57" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="58" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A58" t="s">
-        <v>99</v>
       </c>
       <c r="B58" t="s">
         <v>6</v>
@@ -1490,153 +1496,153 @@
         <v>7</v>
       </c>
       <c r="D58" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="B59" t="s">
-        <v>102</v>
+        <v>6</v>
+      </c>
+      <c r="C59" t="s">
+        <v>7</v>
       </c>
       <c r="D59" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="B60" t="s">
-        <v>23</v>
+        <v>102</v>
       </c>
       <c r="D60" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="B61" t="s">
-        <v>107</v>
-      </c>
-      <c r="C61" t="s">
-        <v>17</v>
+        <v>23</v>
       </c>
       <c r="D61" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
     </row>
     <row r="62" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="B62" t="s">
-        <v>6</v>
+        <v>107</v>
       </c>
       <c r="C62" t="s">
-        <v>7</v>
+        <v>17</v>
       </c>
       <c r="D62" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
     </row>
     <row r="63" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
+        <v>109</v>
+      </c>
+      <c r="B63" t="s">
+        <v>6</v>
+      </c>
+      <c r="C63" t="s">
+        <v>7</v>
+      </c>
+      <c r="D63" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="64" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A64" t="s">
         <v>111</v>
       </c>
-      <c r="B63" t="s">
+      <c r="B64" t="s">
         <v>112</v>
       </c>
-      <c r="C63" t="s">
+      <c r="C64" t="s">
         <v>53</v>
       </c>
-      <c r="D63" t="s">
+      <c r="D64" t="s">
         <v>113</v>
       </c>
     </row>
-    <row r="65" spans="1:4" s="2" customFormat="1" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A65" s="1" t="s">
+    <row r="66" spans="1:4" s="2" customFormat="1" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A66" s="1" t="s">
         <v>114</v>
       </c>
     </row>
-    <row r="66" spans="1:4" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A66" s="2" t="s">
+    <row r="67" spans="1:4" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A67" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B66" s="2" t="s">
+      <c r="B67" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="C66" s="2" t="s">
+      <c r="C67" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="D66" s="2" t="s">
+      <c r="D67" s="2" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="67" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A67" t="s">
+    <row r="68" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A68" t="s">
         <v>115</v>
       </c>
-      <c r="B67" t="s">
+      <c r="B68" t="s">
         <v>116</v>
       </c>
-      <c r="C67" t="s">
+      <c r="C68" t="s">
         <v>117</v>
       </c>
-      <c r="D67" t="s">
+      <c r="D68" t="s">
         <v>118</v>
       </c>
     </row>
-    <row r="68" spans="1:4" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A68" t="s">
+    <row r="69" spans="1:4" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A69" t="s">
         <v>119</v>
       </c>
-      <c r="B68" t="s">
+      <c r="B69" t="s">
         <v>120</v>
       </c>
-      <c r="D68" s="3" t="s">
+      <c r="D69" s="3" t="s">
         <v>121</v>
       </c>
     </row>
-    <row r="70" spans="1:4" s="2" customFormat="1" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A70" s="1" t="s">
+    <row r="71" spans="1:4" s="2" customFormat="1" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A71" s="1" t="s">
         <v>122</v>
       </c>
     </row>
-    <row r="71" spans="1:4" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A71" s="2" t="s">
+    <row r="72" spans="1:4" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A72" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B71" s="2" t="s">
+      <c r="B72" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="C71" s="2" t="s">
+      <c r="C72" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="D71" s="2" t="s">
+      <c r="D72" s="2" t="s">
         <v>4</v>
-      </c>
-    </row>
-    <row r="72" spans="1:4" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A72" t="s">
-        <v>123</v>
-      </c>
-      <c r="B72" t="s">
-        <v>136</v>
-      </c>
-      <c r="C72" t="s">
-        <v>124</v>
-      </c>
-      <c r="D72" s="3" t="s">
-        <v>125</v>
       </c>
     </row>
     <row r="73" spans="1:4" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
-        <v>135</v>
+        <v>123</v>
       </c>
       <c r="B73" t="s">
         <v>136</v>
@@ -1645,59 +1651,73 @@
         <v>124</v>
       </c>
       <c r="D73" s="3" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="74" spans="1:4" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A74" t="s">
+        <v>135</v>
+      </c>
+      <c r="B74" t="s">
+        <v>136</v>
+      </c>
+      <c r="C74" t="s">
+        <v>124</v>
+      </c>
+      <c r="D74" s="3" t="s">
         <v>137</v>
       </c>
     </row>
-    <row r="75" spans="1:4" s="2" customFormat="1" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A75" s="1" t="s">
+    <row r="76" spans="1:4" s="2" customFormat="1" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A76" s="1" t="s">
         <v>126</v>
       </c>
     </row>
-    <row r="76" spans="1:4" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A76" s="2" t="s">
+    <row r="77" spans="1:4" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A77" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B76" s="2" t="s">
+      <c r="B77" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="C76" s="2" t="s">
+      <c r="C77" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="D76" s="2" t="s">
+      <c r="D77" s="2" t="s">
         <v>4</v>
-      </c>
-    </row>
-    <row r="77" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A77" t="s">
-        <v>127</v>
       </c>
     </row>
     <row r="78" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
     <row r="79" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
     </row>
     <row r="80" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="81" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A81" t="s">
         <v>130</v>
       </c>
     </row>
-    <row r="81" spans="1:4" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A81" t="s">
+    <row r="82" spans="1:4" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A82" t="s">
         <v>131</v>
       </c>
-      <c r="B81" t="s">
+      <c r="B82" t="s">
         <v>132</v>
       </c>
-      <c r="C81" t="s">
+      <c r="C82" t="s">
         <v>133</v>
       </c>
-      <c r="D81" s="3" t="s">
+      <c r="D82" s="3" t="s">
         <v>134</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Added script to evaluate NASA polynomials for multiple species
</commit_message>
<xml_diff>
--- a/Master_list.xlsx
+++ b/Master_list.xlsx
@@ -9,12 +9,12 @@
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0" iterateDelta="1E-4"/>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="233" uniqueCount="140">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="237" uniqueCount="142">
   <si>
     <t>Quick operations for one data point</t>
   </si>
@@ -437,6 +437,12 @@
   </si>
   <si>
     <t>For an existing species dictionary, convert adjacency lists for aromatic species to kekulized bond types</t>
+  </si>
+  <si>
+    <t>WIP Evaluate_thermo</t>
+  </si>
+  <si>
+    <t>Takes a chemkin input file that includes both SPECIES and THERMO blocks, and outputs the thermo properties (Cp, H, S and G) of each species by evaluating their NASA polynomials at specified temperatures.</t>
   </si>
 </sst>
 </file>
@@ -486,7 +492,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
@@ -494,6 +500,9 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -863,10 +872,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D82"/>
+  <dimension ref="A1:D83"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A17" sqref="A17"/>
+      <selection activeCell="A21" sqref="A21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -1120,186 +1129,186 @@
         <v>139</v>
       </c>
     </row>
-    <row r="22" spans="1:4" s="2" customFormat="1" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="1" t="s">
+    <row r="21" spans="1:4" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>13</v>
+      </c>
+      <c r="B21" t="s">
+        <v>140</v>
+      </c>
+      <c r="C21" t="s">
+        <v>124</v>
+      </c>
+      <c r="D21" s="5" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" s="2" customFormat="1" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A23" s="1" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="23" spans="1:4" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="2" t="s">
+    <row r="24" spans="1:4" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A24" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B23" s="2" t="s">
+      <c r="B24" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="C23" s="2" t="s">
+      <c r="C24" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="D23" s="2" t="s">
+      <c r="D24" s="2" t="s">
         <v>4</v>
-      </c>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A24" t="s">
-        <v>41</v>
-      </c>
-      <c r="B24" t="s">
-        <v>42</v>
-      </c>
-      <c r="C24" t="s">
-        <v>17</v>
-      </c>
-      <c r="D24" t="s">
-        <v>43</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="B25" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="C25" t="s">
         <v>17</v>
       </c>
       <c r="D25" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>44</v>
+      </c>
+      <c r="B26" t="s">
+        <v>45</v>
+      </c>
+      <c r="C26" t="s">
+        <v>17</v>
+      </c>
+      <c r="D26" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="27" spans="1:4" s="2" customFormat="1" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="1" t="s">
+    <row r="28" spans="1:4" s="2" customFormat="1" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A28" s="1" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="28" spans="1:4" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="2" t="s">
+    <row r="29" spans="1:4" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A29" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B28" s="2" t="s">
+      <c r="B29" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="C28" s="2" t="s">
+      <c r="C29" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="D28" s="2" t="s">
+      <c r="D29" s="2" t="s">
         <v>4</v>
-      </c>
-    </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A29" t="s">
-        <v>48</v>
-      </c>
-      <c r="B29" t="s">
-        <v>49</v>
-      </c>
-      <c r="C29" t="s">
-        <v>50</v>
-      </c>
-      <c r="D29" t="s">
-        <v>51</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="B30" t="s">
-        <v>23</v>
+        <v>49</v>
       </c>
       <c r="C30" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="D30" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="B31" t="s">
-        <v>56</v>
+        <v>23</v>
       </c>
       <c r="C31" t="s">
-        <v>17</v>
+        <v>53</v>
       </c>
       <c r="D31" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="B32" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="C32" t="s">
-        <v>60</v>
+        <v>17</v>
       </c>
       <c r="D32" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="B33" t="s">
-        <v>63</v>
+        <v>59</v>
+      </c>
+      <c r="C33" t="s">
+        <v>60</v>
       </c>
       <c r="D33" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
+        <v>62</v>
+      </c>
+      <c r="B34" t="s">
+        <v>63</v>
+      </c>
+      <c r="D34" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
         <v>65</v>
       </c>
-      <c r="B34" t="s">
+      <c r="B35" t="s">
         <v>66</v>
       </c>
-      <c r="D34" t="s">
+      <c r="D35" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="36" spans="1:4" s="2" customFormat="1" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A36" s="1" t="s">
+    <row r="37" spans="1:4" s="2" customFormat="1" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A37" s="1" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="37" spans="1:4" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A37" s="2" t="s">
+    <row r="38" spans="1:4" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A38" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B37" s="2" t="s">
+      <c r="B38" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="C37" s="2" t="s">
+      <c r="C38" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="D37" s="2" t="s">
+      <c r="D38" s="2" t="s">
         <v>4</v>
-      </c>
-    </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A38" t="s">
-        <v>69</v>
-      </c>
-      <c r="B38" t="s">
-        <v>6</v>
-      </c>
-      <c r="C38" t="s">
-        <v>7</v>
-      </c>
-      <c r="D38" t="s">
-        <v>70</v>
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>5</v>
+        <v>69</v>
       </c>
       <c r="B39" t="s">
         <v>6</v>
@@ -1308,153 +1317,153 @@
         <v>7</v>
       </c>
       <c r="D39" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>72</v>
+        <v>5</v>
       </c>
       <c r="B40" t="s">
-        <v>63</v>
+        <v>6</v>
+      </c>
+      <c r="C40" t="s">
+        <v>7</v>
       </c>
       <c r="D40" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="B41" t="s">
         <v>63</v>
       </c>
       <c r="D41" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
+        <v>74</v>
+      </c>
+      <c r="B42" t="s">
+        <v>63</v>
+      </c>
+      <c r="D42" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A43" t="s">
         <v>76</v>
       </c>
-      <c r="B42" t="s">
+      <c r="B43" t="s">
         <v>56</v>
       </c>
-      <c r="C42" t="s">
+      <c r="C43" t="s">
         <v>7</v>
       </c>
-      <c r="D42" t="s">
+      <c r="D43" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="44" spans="1:4" s="2" customFormat="1" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A44" s="1" t="s">
+    <row r="45" spans="1:4" s="2" customFormat="1" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A45" s="1" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="45" spans="1:4" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A45" s="2" t="s">
+    <row r="46" spans="1:4" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A46" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B45" s="2" t="s">
+      <c r="B46" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="C45" s="2" t="s">
+      <c r="C46" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="D45" s="2" t="s">
+      <c r="D46" s="2" t="s">
         <v>4</v>
-      </c>
-    </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A46" t="s">
-        <v>79</v>
-      </c>
-      <c r="B46" t="s">
-        <v>30</v>
-      </c>
-      <c r="C46" t="s">
-        <v>7</v>
-      </c>
-      <c r="D46" t="s">
-        <v>80</v>
       </c>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="B47" t="s">
         <v>30</v>
       </c>
       <c r="C47" t="s">
-        <v>17</v>
+        <v>7</v>
       </c>
       <c r="D47" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
+        <v>81</v>
+      </c>
+      <c r="B48" t="s">
+        <v>30</v>
+      </c>
+      <c r="C48" t="s">
+        <v>17</v>
+      </c>
+      <c r="D48" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A49" t="s">
         <v>83</v>
       </c>
-      <c r="B48" t="s">
+      <c r="B49" t="s">
         <v>84</v>
       </c>
-      <c r="C48" t="s">
+      <c r="C49" t="s">
         <v>85</v>
       </c>
-      <c r="D48" t="s">
+      <c r="D49" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="50" spans="1:4" s="2" customFormat="1" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A50" s="1" t="s">
+    <row r="51" spans="1:4" s="2" customFormat="1" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A51" s="1" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="51" spans="1:4" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A51" s="2" t="s">
+    <row r="52" spans="1:4" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A52" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B51" s="2" t="s">
+      <c r="B52" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="C51" s="2" t="s">
+      <c r="C52" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="D51" s="2" t="s">
+      <c r="D52" s="2" t="s">
         <v>4</v>
-      </c>
-    </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A52" t="s">
-        <v>88</v>
-      </c>
-      <c r="B52" t="s">
-        <v>89</v>
-      </c>
-      <c r="D52" t="s">
-        <v>90</v>
       </c>
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="B53" t="s">
-        <v>92</v>
-      </c>
-      <c r="C53" t="s">
-        <v>17</v>
+        <v>89</v>
       </c>
       <c r="D53" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="B54" t="s">
         <v>92</v>
@@ -1463,45 +1472,45 @@
         <v>17</v>
       </c>
       <c r="D54" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A55" t="s">
+        <v>94</v>
+      </c>
+      <c r="B55" t="s">
+        <v>92</v>
+      </c>
+      <c r="C55" t="s">
+        <v>17</v>
+      </c>
+      <c r="D55" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="56" spans="1:4" s="2" customFormat="1" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A56" s="1" t="s">
+    <row r="57" spans="1:4" s="2" customFormat="1" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A57" s="1" t="s">
         <v>96</v>
       </c>
     </row>
-    <row r="57" spans="1:4" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A57" s="2" t="s">
+    <row r="58" spans="1:4" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A58" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B57" s="2" t="s">
+      <c r="B58" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="C57" s="2" t="s">
+      <c r="C58" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="D57" s="2" t="s">
+      <c r="D58" s="2" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="58" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A58" s="4" t="s">
+    <row r="59" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A59" s="4" t="s">
         <v>97</v>
-      </c>
-      <c r="B58" t="s">
-        <v>6</v>
-      </c>
-      <c r="C58" t="s">
-        <v>7</v>
-      </c>
-      <c r="D58" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="59" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A59" t="s">
-        <v>99</v>
       </c>
       <c r="B59" t="s">
         <v>6</v>
@@ -1510,153 +1519,153 @@
         <v>7</v>
       </c>
       <c r="D59" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="B60" t="s">
-        <v>102</v>
+        <v>6</v>
+      </c>
+      <c r="C60" t="s">
+        <v>7</v>
       </c>
       <c r="D60" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="B61" t="s">
-        <v>23</v>
+        <v>102</v>
       </c>
       <c r="D61" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
     </row>
     <row r="62" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="B62" t="s">
-        <v>107</v>
-      </c>
-      <c r="C62" t="s">
-        <v>17</v>
+        <v>23</v>
       </c>
       <c r="D62" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
     </row>
     <row r="63" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="B63" t="s">
-        <v>6</v>
+        <v>107</v>
       </c>
       <c r="C63" t="s">
-        <v>7</v>
+        <v>17</v>
       </c>
       <c r="D63" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
     </row>
     <row r="64" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
+        <v>109</v>
+      </c>
+      <c r="B64" t="s">
+        <v>6</v>
+      </c>
+      <c r="C64" t="s">
+        <v>7</v>
+      </c>
+      <c r="D64" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="65" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A65" t="s">
         <v>111</v>
       </c>
-      <c r="B64" t="s">
+      <c r="B65" t="s">
         <v>112</v>
       </c>
-      <c r="C64" t="s">
+      <c r="C65" t="s">
         <v>53</v>
       </c>
-      <c r="D64" t="s">
+      <c r="D65" t="s">
         <v>113</v>
       </c>
     </row>
-    <row r="66" spans="1:4" s="2" customFormat="1" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A66" s="1" t="s">
+    <row r="67" spans="1:4" s="2" customFormat="1" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A67" s="1" t="s">
         <v>114</v>
       </c>
     </row>
-    <row r="67" spans="1:4" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A67" s="2" t="s">
+    <row r="68" spans="1:4" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A68" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B67" s="2" t="s">
+      <c r="B68" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="C67" s="2" t="s">
+      <c r="C68" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="D67" s="2" t="s">
+      <c r="D68" s="2" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="68" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A68" t="s">
+    <row r="69" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A69" t="s">
         <v>115</v>
       </c>
-      <c r="B68" t="s">
+      <c r="B69" t="s">
         <v>116</v>
       </c>
-      <c r="C68" t="s">
+      <c r="C69" t="s">
         <v>117</v>
       </c>
-      <c r="D68" t="s">
+      <c r="D69" t="s">
         <v>118</v>
       </c>
     </row>
-    <row r="69" spans="1:4" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A69" t="s">
+    <row r="70" spans="1:4" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A70" t="s">
         <v>119</v>
       </c>
-      <c r="B69" t="s">
+      <c r="B70" t="s">
         <v>120</v>
       </c>
-      <c r="D69" s="3" t="s">
+      <c r="D70" s="3" t="s">
         <v>121</v>
       </c>
     </row>
-    <row r="71" spans="1:4" s="2" customFormat="1" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A71" s="1" t="s">
+    <row r="72" spans="1:4" s="2" customFormat="1" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A72" s="1" t="s">
         <v>122</v>
       </c>
     </row>
-    <row r="72" spans="1:4" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A72" s="2" t="s">
+    <row r="73" spans="1:4" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A73" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B72" s="2" t="s">
+      <c r="B73" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="C72" s="2" t="s">
+      <c r="C73" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="D72" s="2" t="s">
+      <c r="D73" s="2" t="s">
         <v>4</v>
-      </c>
-    </row>
-    <row r="73" spans="1:4" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A73" t="s">
-        <v>123</v>
-      </c>
-      <c r="B73" t="s">
-        <v>136</v>
-      </c>
-      <c r="C73" t="s">
-        <v>124</v>
-      </c>
-      <c r="D73" s="3" t="s">
-        <v>125</v>
       </c>
     </row>
     <row r="74" spans="1:4" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
-        <v>135</v>
+        <v>123</v>
       </c>
       <c r="B74" t="s">
         <v>136</v>
@@ -1665,64 +1674,78 @@
         <v>124</v>
       </c>
       <c r="D74" s="3" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="75" spans="1:4" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A75" t="s">
+        <v>135</v>
+      </c>
+      <c r="B75" t="s">
+        <v>136</v>
+      </c>
+      <c r="C75" t="s">
+        <v>124</v>
+      </c>
+      <c r="D75" s="3" t="s">
         <v>137</v>
       </c>
     </row>
-    <row r="76" spans="1:4" s="2" customFormat="1" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A76" s="1" t="s">
+    <row r="77" spans="1:4" s="2" customFormat="1" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A77" s="1" t="s">
         <v>126</v>
       </c>
     </row>
-    <row r="77" spans="1:4" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A77" s="2" t="s">
+    <row r="78" spans="1:4" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A78" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B77" s="2" t="s">
+      <c r="B78" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="C77" s="2" t="s">
+      <c r="C78" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="D77" s="2" t="s">
+      <c r="D78" s="2" t="s">
         <v>4</v>
-      </c>
-    </row>
-    <row r="78" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A78" t="s">
-        <v>127</v>
       </c>
     </row>
     <row r="79" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
     <row r="80" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
     </row>
     <row r="81" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="82" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A82" t="s">
         <v>130</v>
       </c>
     </row>
-    <row r="82" spans="1:4" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A82" t="s">
+    <row r="83" spans="1:4" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A83" t="s">
         <v>131</v>
       </c>
-      <c r="B82" t="s">
+      <c r="B83" t="s">
         <v>132</v>
       </c>
-      <c r="C82" t="s">
+      <c r="C83" t="s">
         <v>133</v>
       </c>
-      <c r="D82" s="3" t="s">
+      <c r="D83" s="3" t="s">
         <v>134</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
-  <pageSetup paperSize="0" scale="0" firstPageNumber="0" orientation="portrait" usePrinterDefaults="0" horizontalDpi="0" verticalDpi="0" copies="0"/>
+  <pageSetup firstPageNumber="0" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>